<commit_message>
Update the readme for the docstring additions
</commit_message>
<xml_diff>
--- a/src/api.xlsx
+++ b/src/api.xlsx
@@ -3485,18 +3485,6 @@
     <t>Set the characters used for White space in the command string. Default in blank and Tab.</t>
   </si>
   <si>
-    <t>Get the string containing the characters for quoting in OpenDSS scripts. Matching pairs defined in EndQuote. Default is "([{.</t>
-  </si>
-  <si>
-    <t>Set the string containing the characters for quoting in OpenDSS scripts. Matching pairs defined in EndQuote. Default is "([{.</t>
-  </si>
-  <si>
-    <t>Get the string containing the characters, in order, that match the beginning quote characters in BeginQuote. Default is ")]}.</t>
-  </si>
-  <si>
-    <t>Set the string containing the characters, in order, that match the beginning quote characters in BeginQuote. Default is ")]}.</t>
-  </si>
-  <si>
     <t>Get the string defining hard delimiters used to separate token on the command string. Default is , and =. The =  separates token name from token value. These override whitespace to separate tokens.</t>
   </si>
   <si>
@@ -4650,6 +4638,18 @@
   </si>
   <si>
     <t>Set the power factor value.</t>
+  </si>
+  <si>
+    <t>Set the string containing the characters, in order, that match the beginning quote characters in BeginQuote. Default is \")]}.</t>
+  </si>
+  <si>
+    <t>Get the string containing the characters, in order, that match the beginning quote characters in BeginQuote. Default is \")]}.</t>
+  </si>
+  <si>
+    <t>Set the string containing the characters for quoting in OpenDSS scripts. Matching pairs defined in EndQuote. Default is \"([{.</t>
+  </si>
+  <si>
+    <t>Get the string containing the characters for quoting in OpenDSS scripts. Matching pairs defined in EndQuote. Default is \"([{.</t>
   </si>
 </sst>
 </file>
@@ -4981,8 +4981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I954"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="H525" workbookViewId="0">
+      <selection activeCell="I541" sqref="I541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4991,8 +4991,8 @@
     <col min="4" max="4" width="12.81640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="1"/>
     <col min="6" max="6" width="17.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="68.36328125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="4" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="68.36328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4" style="1" customWidth="1"/>
     <col min="9" max="9" width="59.7265625" style="1" customWidth="1"/>
     <col min="10" max="10" width="42.6328125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="8.7265625" style="1"/>
@@ -14816,7 +14816,7 @@
         <v>"If true, loads are line to line."</v>
       </c>
       <c r="I359" s="1" t="s">
-        <v>1526</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.35">
@@ -14843,7 +14843,7 @@
         <v>"Set whether loads are delta (line to line)."</v>
       </c>
       <c r="I360" s="1" t="s">
-        <v>1527</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.35">
@@ -17052,9 +17052,9 @@
       <c r="F442" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="G442" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G442" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>"Get a variant array of doubles for the P multiplier in the LoadShape."</v>
       </c>
       <c r="I442" s="1" t="s">
         <v>1053</v>
@@ -17080,8 +17080,8 @@
         <v>534</v>
       </c>
       <c r="G443" s="1" t="str">
-        <f>""""&amp;TRIM(I442)&amp;""""</f>
-        <v>"Get a variant array of doubles for the P multiplier in the LoadShape."</v>
+        <f t="shared" si="6"/>
+        <v>"Set a variant array of doubles for the P multiplier in the LoadShape."</v>
       </c>
       <c r="I443" s="1" t="s">
         <v>1054</v>
@@ -17107,8 +17107,8 @@
         <v>535</v>
       </c>
       <c r="G444" s="1" t="str">
-        <f>""""&amp;TRIM(I443)&amp;""""</f>
-        <v>"Set a variant array of doubles for the P multiplier in the LoadShape."</v>
+        <f t="shared" si="6"/>
+        <v>"Get a variant array of doubles for the Q multiplier in the LoadShape."</v>
       </c>
       <c r="I444" s="1" t="s">
         <v>1055</v>
@@ -17134,8 +17134,8 @@
         <v>535</v>
       </c>
       <c r="G445" s="1" t="str">
-        <f>""""&amp;TRIM(I444)&amp;""""</f>
-        <v>"Get a variant array of doubles for the Q multiplier in the LoadShape."</v>
+        <f t="shared" si="6"/>
+        <v>"Set a variant array of doubles for the Q multiplier in the LoadShape."</v>
       </c>
       <c r="I445" s="1" t="s">
         <v>1056</v>
@@ -17161,8 +17161,8 @@
         <v>536</v>
       </c>
       <c r="G446" s="1" t="str">
-        <f>""""&amp;TRIM(I445)&amp;""""</f>
-        <v>"Set a variant array of doubles for the Q multiplier in the LoadShape."</v>
+        <f t="shared" si="6"/>
+        <v>"Get a time array in hours corresponding to P and Q multipliers when the Interval = 0."</v>
       </c>
       <c r="I446" s="1" t="s">
         <v>1057</v>
@@ -17188,8 +17188,8 @@
         <v>536</v>
       </c>
       <c r="G447" s="1" t="str">
-        <f>""""&amp;TRIM(I446)&amp;""""</f>
-        <v>"Get a time array in hours corresponding to P and Q multipliers when the Interval = 0."</v>
+        <f t="shared" si="6"/>
+        <v>"Set a time array in hours corresponding to P and Q multipliers when the Interval = 0."</v>
       </c>
       <c r="I447" s="1" t="s">
         <v>1058</v>
@@ -17215,8 +17215,8 @@
         <v>113</v>
       </c>
       <c r="G448" s="1" t="str">
-        <f>""""&amp;TRIM(I447)&amp;""""</f>
-        <v>"Set a time array in hours corresponding to P and Q multipliers when the Interval = 0."</v>
+        <f t="shared" si="6"/>
+        <v>"Set the first Energy Meter active. Returns 0 if no monitors."</v>
       </c>
       <c r="I448" s="1" t="s">
         <v>1059</v>
@@ -19024,7 +19024,7 @@
         <v>1130</v>
       </c>
       <c r="G515" s="1" t="str">
-        <f t="shared" ref="G515:G568" si="8">""""&amp;TRIM(I515)&amp;""""</f>
+        <f t="shared" ref="G515:G578" si="8">""""&amp;TRIM(I515)&amp;""""</f>
         <v>"The size of each record in ByteStream."</v>
       </c>
       <c r="I515" s="1" t="s">
@@ -19104,6 +19104,10 @@
       <c r="F518" s="1" t="s">
         <v>583</v>
       </c>
+      <c r="G518" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>"Set the terminal number of element being monitored."</v>
+      </c>
       <c r="I518" s="1" t="s">
         <v>1129</v>
       </c>
@@ -19128,8 +19132,8 @@
         <v>584</v>
       </c>
       <c r="G519" s="1" t="str">
-        <f>""""&amp;TRIM(I518)&amp;""""</f>
-        <v>"Set the terminal number of element being monitored."</v>
+        <f t="shared" si="8"/>
+        <v>"The name of the CSV file associated with active monitor."</v>
       </c>
       <c r="I519" s="1" t="s">
         <v>1131</v>
@@ -19645,7 +19649,7 @@
         <v>"Return next parameter as a string."</v>
       </c>
       <c r="I538" s="1" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="539" spans="1:9" x14ac:dyDescent="0.35">
@@ -19723,10 +19727,10 @@
       </c>
       <c r="G541" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>"Get the string containing the characters for quoting in OpenDSS scripts. Matching pairs defined in EndQuote. Default is "([{."</v>
+        <v>"Get the string containing the characters for quoting in OpenDSS scripts. Matching pairs defined in EndQuote. Default is \"([{."</v>
       </c>
       <c r="I541" s="1" t="s">
-        <v>1151</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="542" spans="1:9" x14ac:dyDescent="0.35">
@@ -19750,10 +19754,10 @@
       </c>
       <c r="G542" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>"Set the string containing the characters for quoting in OpenDSS scripts. Matching pairs defined in EndQuote. Default is "([{."</v>
+        <v>"Set the string containing the characters for quoting in OpenDSS scripts. Matching pairs defined in EndQuote. Default is \"([{."</v>
       </c>
       <c r="I542" s="1" t="s">
-        <v>1152</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="543" spans="1:9" x14ac:dyDescent="0.35">
@@ -19777,10 +19781,10 @@
       </c>
       <c r="G543" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>"Get the string containing the characters, in order, that match the beginning quote characters in BeginQuote. Default is ")]}."</v>
+        <v>"Get the string containing the characters, in order, that match the beginning quote characters in BeginQuote. Default is \")]}."</v>
       </c>
       <c r="I543" s="1" t="s">
-        <v>1153</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="544" spans="1:9" x14ac:dyDescent="0.35">
@@ -19804,10 +19808,10 @@
       </c>
       <c r="G544" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>"Set the string containing the characters, in order, that match the beginning quote characters in BeginQuote. Default is ")]}."</v>
+        <v>"Set the string containing the characters, in order, that match the beginning quote characters in BeginQuote. Default is \")]}."</v>
       </c>
       <c r="I544" s="1" t="s">
-        <v>1154</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="545" spans="1:9" x14ac:dyDescent="0.35">
@@ -19834,7 +19838,7 @@
         <v>"Get the string defining hard delimiters used to separate token on the command string. Default is , and =. The = separates token name from token value. These override whitespace to separate tokens."</v>
       </c>
       <c r="I545" s="1" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="546" spans="1:9" x14ac:dyDescent="0.35">
@@ -19861,7 +19865,7 @@
         <v>"Set the string defining hard delimiters used to separate token on the command string. Default is , and =. The = separates token name from token value. These override whitespace to separate tokens."</v>
       </c>
       <c r="I546" s="1" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="547" spans="1:9" x14ac:dyDescent="0.35">
@@ -19888,7 +19892,7 @@
         <v>"Returns token as vector of doubles. For parsing quoted array syntax."</v>
       </c>
       <c r="I547" s="1" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="548" spans="1:9" x14ac:dyDescent="0.35">
@@ -19915,7 +19919,7 @@
         <v>"Use this property to parse a Matrix token in OpenDSS format. Returns square matrix of order specified. Order same as default fortran order: column by column."</v>
       </c>
       <c r="I548" s="1" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="549" spans="1:9" x14ac:dyDescent="0.35">
@@ -19942,7 +19946,7 @@
         <v>"Use this property to parse a Matrix token in lower triangular form. Symmetry is forced."</v>
       </c>
       <c r="I549" s="1" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="550" spans="1:9" x14ac:dyDescent="0.35">
@@ -19969,7 +19973,7 @@
         <v>"Get number of PDElements in active circuit."</v>
       </c>
       <c r="I550" s="1" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="551" spans="1:9" x14ac:dyDescent="0.35">
@@ -19996,7 +20000,7 @@
         <v>"Set the first enabled PD element to be the active element. Returns 0 if none found."</v>
       </c>
       <c r="I551" s="1" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="552" spans="1:9" x14ac:dyDescent="0.35">
@@ -20023,7 +20027,7 @@
         <v>"Set the next enabled PD element to be the active element. Returns 0 if none found."</v>
       </c>
       <c r="I552" s="1" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="553" spans="1:9" x14ac:dyDescent="0.35">
@@ -20050,7 +20054,7 @@
         <v>"returns 1 if the PD element should be treated as a shunt element rather than a series element. Applies to capacitor and reactor elements in particular."</v>
       </c>
       <c r="I553" s="1" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="554" spans="1:9" x14ac:dyDescent="0.35">
@@ -20077,7 +20081,7 @@
         <v>"Get the number of customers in this branch."</v>
       </c>
       <c r="I554" s="1" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="555" spans="1:9" x14ac:dyDescent="0.35">
@@ -20104,7 +20108,7 @@
         <v>"Get the total number of customers from this branch to the end of the zone."</v>
       </c>
       <c r="I555" s="1" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="556" spans="1:9" x14ac:dyDescent="0.35">
@@ -20131,7 +20135,7 @@
         <v>"Set the parent PD element to be the active circuit element. Returns 0 if no more elements upline."</v>
       </c>
       <c r="I556" s="1" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="557" spans="1:9" x14ac:dyDescent="0.35">
@@ -20158,7 +20162,7 @@
         <v>"Get the number of the terminal of active PD element that is on the "from" side. This is set after the meter zone is determined."</v>
       </c>
       <c r="I557" s="1" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="558" spans="1:9" x14ac:dyDescent="0.35">
@@ -20185,7 +20189,7 @@
         <v>"Get the integer ID of the feeder section that this PDElement branch is part of."</v>
       </c>
       <c r="I558" s="1" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="559" spans="1:9" x14ac:dyDescent="0.35">
@@ -20212,7 +20216,7 @@
         <v>"Get the number of failures per year. For LINE elements: Number of failures per unit length per year."</v>
       </c>
       <c r="I559" s="1" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="560" spans="1:9" x14ac:dyDescent="0.35">
@@ -20239,7 +20243,7 @@
         <v>"Set the number of failures per year. For LINE elements: Number of failures per unit length per year."</v>
       </c>
       <c r="I560" s="1" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="561" spans="1:9" x14ac:dyDescent="0.35">
@@ -20266,7 +20270,7 @@
         <v>"Get the percent of faults that are permanent (require repair). Otherwise, fault is assumed to be transient/temporary."</v>
       </c>
       <c r="I561" s="1" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="562" spans="1:9" x14ac:dyDescent="0.35">
@@ -20293,7 +20297,7 @@
         <v>"Set the percent of faults that are permanent (require repair). Otherwise, fault is assumed to be transient/temporary."</v>
       </c>
       <c r="I562" s="1" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="563" spans="1:9" x14ac:dyDescent="0.35">
@@ -20320,7 +20324,7 @@
         <v>"Get the failure rate for this branch. Faults per year including length of line."</v>
       </c>
       <c r="I563" s="1" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="564" spans="1:9" x14ac:dyDescent="0.35">
@@ -20347,7 +20351,7 @@
         <v>"Get the accumulated failure rate for this branch on down line."</v>
       </c>
       <c r="I564" s="1" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="565" spans="1:9" x14ac:dyDescent="0.35">
@@ -20374,7 +20378,7 @@
         <v>"Get the average time to repair a permanent fault on this branch, hours."</v>
       </c>
       <c r="I565" s="1" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="566" spans="1:9" x14ac:dyDescent="0.35">
@@ -20401,7 +20405,7 @@
         <v>"Get the total miles of line from this element to the end of the zone. For recloser siting algorithm."</v>
       </c>
       <c r="I566" s="1" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="567" spans="1:9" x14ac:dyDescent="0.35">
@@ -20415,7 +20419,7 @@
         <v>612</v>
       </c>
       <c r="D567" s="1" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="E567" s="1">
         <v>0</v>
@@ -20428,7 +20432,7 @@
         <v>"Get the name of the active PDElement, returns null string if active element id not PDElement."</v>
       </c>
       <c r="I567" s="1" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="568" spans="1:9" x14ac:dyDescent="0.35">
@@ -20442,7 +20446,7 @@
         <v>612</v>
       </c>
       <c r="D568" s="1" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="E568" s="1">
         <v>1</v>
@@ -20455,7 +20459,7 @@
         <v>"Set the name of the active PDElement, returns null string if active element id not PDElement."</v>
       </c>
       <c r="I568" s="1" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="569" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -20478,11 +20482,11 @@
         <v>116</v>
       </c>
       <c r="G569" s="1" t="str">
-        <f>""""&amp;TRIM(I581)&amp;""""</f>
-        <v>"Get number of Reclosers in active circuit."</v>
+        <f t="shared" si="8"/>
+        <v>"The number of PVSystem objects currently defined in the active circuit."</v>
       </c>
       <c r="I569" s="5" t="s">
-        <v>1528</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="570" spans="1:9" x14ac:dyDescent="0.35">
@@ -20505,11 +20509,11 @@
         <v>113</v>
       </c>
       <c r="G570" s="1" t="str">
-        <f>""""&amp;TRIM(I582)&amp;""""</f>
-        <v>"Set first recloser to be active Circuit Element. Returns 0 if none."</v>
+        <f t="shared" si="8"/>
+        <v>"Set the first PVSystem to be active; returns 0 if none."</v>
       </c>
       <c r="I570" s="5" t="s">
-        <v>1529</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="571" spans="1:9" x14ac:dyDescent="0.35">
@@ -20532,11 +20536,11 @@
         <v>114</v>
       </c>
       <c r="G571" s="1" t="str">
-        <f>""""&amp;TRIM(I583)&amp;""""</f>
-        <v>"Set next recloser to be active Circuit Element. Returns 0 if none."</v>
+        <f t="shared" si="8"/>
+        <v>"Set the next PVSystem to be active; returns 0 if none."</v>
       </c>
       <c r="I571" s="5" t="s">
-        <v>1530</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="572" spans="1:9" x14ac:dyDescent="0.35">
@@ -20559,11 +20563,11 @@
         <v>444</v>
       </c>
       <c r="G572" s="1" t="str">
-        <f>""""&amp;TRIM(I584)&amp;""""</f>
-        <v>"Get the terminal number of Monitored Object for the Recloser."</v>
+        <f t="shared" si="8"/>
+        <v>"Get the active PVSystem by index; 1..Count."</v>
       </c>
       <c r="I572" s="5" t="s">
-        <v>1531</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="573" spans="1:9" x14ac:dyDescent="0.35">
@@ -20586,11 +20590,11 @@
         <v>444</v>
       </c>
       <c r="G573" s="1" t="str">
-        <f>""""&amp;TRIM(I585)&amp;""""</f>
-        <v>"Set the terminal number of Monitored Object for the Recloser."</v>
+        <f t="shared" si="8"/>
+        <v>"Set the active PVSystem by index; 1..Count."</v>
       </c>
       <c r="I573" s="5" t="s">
-        <v>1532</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="574" spans="1:9" x14ac:dyDescent="0.35">
@@ -20613,11 +20617,11 @@
         <v>622</v>
       </c>
       <c r="G574" s="1" t="str">
-        <f>""""&amp;TRIM(I586)&amp;""""</f>
-        <v>"Get the terminal of the controlled device being switched by the Recloser."</v>
+        <f t="shared" si="8"/>
+        <v>"Get the present value of the Irradiance property in W/sq-m."</v>
       </c>
       <c r="I574" s="5" t="s">
-        <v>1533</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="575" spans="1:9" x14ac:dyDescent="0.35">
@@ -20640,11 +20644,11 @@
         <v>622</v>
       </c>
       <c r="G575" s="1" t="str">
-        <f>""""&amp;TRIM(I587)&amp;""""</f>
-        <v>"Set the terminal of the controlled device being switched by the Recloser."</v>
+        <f t="shared" si="8"/>
+        <v>"Set the present value of the Irradiance property in W/sq-m."</v>
       </c>
       <c r="I575" s="5" t="s">
-        <v>1534</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="576" spans="1:9" x14ac:dyDescent="0.35">
@@ -20667,11 +20671,11 @@
         <v>150</v>
       </c>
       <c r="G576" s="1" t="str">
-        <f>""""&amp;TRIM(I588)&amp;""""</f>
-        <v>"Get the number of fast shots."</v>
+        <f t="shared" si="8"/>
+        <v>"Get the kW output."</v>
       </c>
       <c r="I576" s="5" t="s">
-        <v>1535</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="577" spans="1:9" x14ac:dyDescent="0.35">
@@ -20694,11 +20698,11 @@
         <v>149</v>
       </c>
       <c r="G577" s="1" t="str">
-        <f>""""&amp;TRIM(I589)&amp;""""</f>
-        <v>"Set the number of fast shots."</v>
+        <f t="shared" si="8"/>
+        <v>"Get the kvar value."</v>
       </c>
       <c r="I577" s="5" t="s">
-        <v>1536</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="578" spans="1:9" x14ac:dyDescent="0.35">
@@ -20721,11 +20725,11 @@
         <v>149</v>
       </c>
       <c r="G578" s="1" t="str">
-        <f>""""&amp;TRIM(I590)&amp;""""</f>
-        <v>"Get the number of shots to lockout (fast + delayed)."</v>
+        <f t="shared" si="8"/>
+        <v>"Set the kvar value."</v>
       </c>
       <c r="I578" s="5" t="s">
-        <v>1537</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="579" spans="1:9" x14ac:dyDescent="0.35">
@@ -20748,11 +20752,11 @@
         <v>623</v>
       </c>
       <c r="G579" s="1" t="str">
-        <f>""""&amp;TRIM(I591)&amp;""""</f>
-        <v>"Set the number of shots to lockout (fast + delayed)."</v>
+        <f t="shared" ref="G579:G642" si="9">""""&amp;TRIM(I579)&amp;""""</f>
+        <v>"Get the power factor value."</v>
       </c>
       <c r="I579" s="5" t="s">
-        <v>1538</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="580" spans="1:9" x14ac:dyDescent="0.35">
@@ -20775,11 +20779,11 @@
         <v>623</v>
       </c>
       <c r="G580" s="1" t="str">
-        <f>""""&amp;TRIM(I592)&amp;""""</f>
-        <v>"Open recloser's controlled element and lock out the recloser."</v>
+        <f t="shared" si="9"/>
+        <v>"Set the power factor value."</v>
       </c>
       <c r="I580" s="5" t="s">
-        <v>1539</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="581" spans="1:9" x14ac:dyDescent="0.35">
@@ -20802,11 +20806,11 @@
         <v>116</v>
       </c>
       <c r="G581" s="1" t="str">
-        <f>""""&amp;TRIM(I593)&amp;""""</f>
-        <v>"Close the switched object controlled by the recloser. Resets recloser to first operation."</v>
+        <f t="shared" si="9"/>
+        <v>"Get number of Reclosers in active circuit."</v>
       </c>
       <c r="I581" s="1" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="582" spans="1:9" x14ac:dyDescent="0.35">
@@ -20829,11 +20833,11 @@
         <v>113</v>
       </c>
       <c r="G582" s="1" t="str">
-        <f>""""&amp;TRIM(I594)&amp;""""</f>
-        <v>"Get the active recloser by index into the recloser list. 1..Count."</v>
+        <f t="shared" si="9"/>
+        <v>"Set first recloser to be active Circuit Element. Returns 0 if none."</v>
       </c>
       <c r="I582" s="1" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="583" spans="1:9" x14ac:dyDescent="0.35">
@@ -20856,11 +20860,11 @@
         <v>114</v>
       </c>
       <c r="G583" s="1" t="str">
-        <f>""""&amp;TRIM(I595)&amp;""""</f>
-        <v>"Set the active recloser by index into the recloser list. 1..Count."</v>
+        <f t="shared" si="9"/>
+        <v>"Set next recloser to be active Circuit Element. Returns 0 if none."</v>
       </c>
       <c r="I583" s="1" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="584" spans="1:9" x14ac:dyDescent="0.35">
@@ -20882,12 +20886,12 @@
       <c r="F584" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G584" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G584" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Get the terminal number of Monitored Object for the Recloser."</v>
       </c>
       <c r="I584" s="1" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="585" spans="1:9" x14ac:dyDescent="0.35">
@@ -20909,12 +20913,12 @@
       <c r="F585" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="G585" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G585" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Set the terminal number of Monitored Object for the Recloser."</v>
       </c>
       <c r="I585" s="1" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="586" spans="1:9" x14ac:dyDescent="0.35">
@@ -20936,12 +20940,12 @@
       <c r="F586" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="G586" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G586" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Get the terminal of the controlled device being switched by the Recloser."</v>
       </c>
       <c r="I586" s="1" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="587" spans="1:9" x14ac:dyDescent="0.35">
@@ -20963,12 +20967,12 @@
       <c r="F587" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="G587" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G587" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Set the terminal of the controlled device being switched by the Recloser."</v>
       </c>
       <c r="I587" s="1" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="588" spans="1:9" x14ac:dyDescent="0.35">
@@ -20990,12 +20994,12 @@
       <c r="F588" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="G588" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G588" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Get the number of fast shots."</v>
       </c>
       <c r="I588" s="1" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="589" spans="1:9" x14ac:dyDescent="0.35">
@@ -21017,12 +21021,12 @@
       <c r="F589" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="G589" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G589" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Set the number of fast shots."</v>
       </c>
       <c r="I589" s="1" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="590" spans="1:9" x14ac:dyDescent="0.35">
@@ -21044,12 +21048,12 @@
       <c r="F590" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="G590" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G590" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Get the number of shots to lockout (fast + delayed)."</v>
       </c>
       <c r="I590" s="1" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.35">
@@ -21071,12 +21075,12 @@
       <c r="F591" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="G591" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G591" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Set the number of shots to lockout (fast + delayed)."</v>
       </c>
       <c r="I591" s="1" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="592" spans="1:9" x14ac:dyDescent="0.35">
@@ -21098,12 +21102,12 @@
       <c r="F592" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G592" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G592" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Open recloser's controlled element and lock out the recloser."</v>
       </c>
       <c r="I592" s="1" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="593" spans="1:9" x14ac:dyDescent="0.35">
@@ -21125,12 +21129,12 @@
       <c r="F593" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G593" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G593" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Close the switched object controlled by the recloser. Resets recloser to first operation."</v>
       </c>
       <c r="I593" s="1" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="594" spans="1:9" x14ac:dyDescent="0.35">
@@ -21152,12 +21156,12 @@
       <c r="F594" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="G594" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G594" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Get the active recloser by index into the recloser list. 1..Count."</v>
       </c>
       <c r="I594" s="1" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="595" spans="1:9" x14ac:dyDescent="0.35">
@@ -21179,12 +21183,12 @@
       <c r="F595" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="G595" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G595" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>"Set the active recloser by index into the recloser list. 1..Count."</v>
       </c>
       <c r="I595" s="1" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="596" spans="1:9" x14ac:dyDescent="0.35">
@@ -21207,11 +21211,11 @@
         <v>630</v>
       </c>
       <c r="G596" s="1" t="str">
-        <f t="shared" ref="G596:G643" si="9">""""&amp;TRIM(I596)&amp;""""</f>
+        <f t="shared" si="9"/>
         <v>"Get the phase trip curve multiplier or actual amps."</v>
       </c>
       <c r="I596" s="1" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="597" spans="1:9" x14ac:dyDescent="0.35">
@@ -21238,7 +21242,7 @@
         <v>"Set the phase trip curve multiplier or actual amps."</v>
       </c>
       <c r="I597" s="1" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="598" spans="1:9" x14ac:dyDescent="0.35">
@@ -21265,7 +21269,7 @@
         <v>"Get the phase instantaneous curve multiplier or actual amps."</v>
       </c>
       <c r="I598" s="1" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="599" spans="1:9" x14ac:dyDescent="0.35">
@@ -21292,7 +21296,7 @@
         <v>"Set the phase instantaneous curve multiplier or actual amps."</v>
       </c>
       <c r="I599" s="1" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="600" spans="1:9" x14ac:dyDescent="0.35">
@@ -21319,7 +21323,7 @@
         <v>"Get the ground (3I0) trip multiplier or actual amps."</v>
       </c>
       <c r="I600" s="1" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="601" spans="1:9" x14ac:dyDescent="0.35">
@@ -21346,7 +21350,7 @@
         <v>"Set the ground (3I0) trip multiplier or actual amps."</v>
       </c>
       <c r="I601" s="1" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="602" spans="1:9" x14ac:dyDescent="0.35">
@@ -21373,7 +21377,7 @@
         <v>"Get the ground (3I0) instantaneous trip setting - curve multiplier or actual amps."</v>
       </c>
       <c r="I602" s="1" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="603" spans="1:9" x14ac:dyDescent="0.35">
@@ -21400,7 +21404,7 @@
         <v>"Set the ground (3I0) instantaneous trip setting - curve multiplier or actual amps."</v>
       </c>
       <c r="I603" s="1" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="604" spans="1:9" x14ac:dyDescent="0.35">
@@ -21427,7 +21431,7 @@
         <v>"Get the name of the active Recloser Object."</v>
       </c>
       <c r="I604" s="1" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="605" spans="1:9" x14ac:dyDescent="0.35">
@@ -21454,7 +21458,7 @@
         <v>"Set the name of the active Recloser Object."</v>
       </c>
       <c r="I605" s="1" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="606" spans="1:9" x14ac:dyDescent="0.35">
@@ -21481,7 +21485,7 @@
         <v>"Get the full name of object this Recloser is monitoring."</v>
       </c>
       <c r="I606" s="1" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="607" spans="1:9" x14ac:dyDescent="0.35">
@@ -21508,7 +21512,7 @@
         <v>"Set the full name of object this Recloser is monitoring."</v>
       </c>
       <c r="I607" s="1" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="608" spans="1:9" x14ac:dyDescent="0.35">
@@ -21535,7 +21539,7 @@
         <v>"Get the full name of the circuit element that is being switched by this Recloser."</v>
       </c>
       <c r="I608" s="1" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="609" spans="1:9" x14ac:dyDescent="0.35">
@@ -21562,7 +21566,7 @@
         <v>"Set the full name of the circuit element that is being switched by this Recloser."</v>
       </c>
       <c r="I609" s="1" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="610" spans="1:9" x14ac:dyDescent="0.35">
@@ -21589,7 +21593,7 @@
         <v>"Get a vector of strings with names of all reclosers in active circuit."</v>
       </c>
       <c r="I610" s="1" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="611" spans="1:9" x14ac:dyDescent="0.35">
@@ -21616,7 +21620,7 @@
         <v>"Get a vector of doubles: reclose intervals (s) between shots."</v>
       </c>
       <c r="I611" s="1" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="612" spans="1:9" x14ac:dyDescent="0.35">
@@ -21643,7 +21647,7 @@
         <v>"Set the first RegControl active. Returns 0 if no more."</v>
       </c>
       <c r="I612" s="1" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="613" spans="1:9" x14ac:dyDescent="0.35">
@@ -21670,7 +21674,7 @@
         <v>"Set the next RegControl active. Returns 0 if no more"</v>
       </c>
       <c r="I613" s="1" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="614" spans="1:9" x14ac:dyDescent="0.35">
@@ -21697,7 +21701,7 @@
         <v>"Get the tapped winding number."</v>
       </c>
       <c r="I614" s="1" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="615" spans="1:9" x14ac:dyDescent="0.35">
@@ -21724,7 +21728,7 @@
         <v>"Set the tapped winding number."</v>
       </c>
       <c r="I615" s="1" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="616" spans="1:9" x14ac:dyDescent="0.35">
@@ -21751,7 +21755,7 @@
         <v>"Get the winding number for PT and CT connections."</v>
       </c>
       <c r="I616" s="1" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="617" spans="1:9" x14ac:dyDescent="0.35">
@@ -21778,7 +21782,7 @@
         <v>"Set the winding number for PT and CT connections."</v>
       </c>
       <c r="I617" s="1" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="618" spans="1:9" x14ac:dyDescent="0.35">
@@ -21805,7 +21809,7 @@
         <v>"Get the setting in the reverse direction, usually not applicable to substation transformers."</v>
       </c>
       <c r="I618" s="1" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="619" spans="1:9" x14ac:dyDescent="0.35">
@@ -21832,7 +21836,7 @@
         <v>"Set the different settings for the reverse direction (see Manual for details), usually not applicable to substation transformers."</v>
       </c>
       <c r="I619" s="1" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="620" spans="1:9" x14ac:dyDescent="0.35">
@@ -21859,7 +21863,7 @@
         <v>"Get the inverse time feature. Time delay is inversely adjusted, proportional to the amount of voltage outside the regulator band."</v>
       </c>
       <c r="I620" s="1" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="621" spans="1:9" x14ac:dyDescent="0.35">
@@ -21886,7 +21890,7 @@
         <v>"Set the inverse time feature. Time delay is inversely adjusted, proportional to the amount of voltage outside the regulator band."</v>
       </c>
       <c r="I621" s="1" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="622" spans="1:9" x14ac:dyDescent="0.35">
@@ -21913,7 +21917,7 @@
         <v>"Get the maximum tap change per iteration in STATIC solution mode. 1 is more realistic, 16 is the default for faster solution."</v>
       </c>
       <c r="I622" s="1" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="623" spans="1:9" x14ac:dyDescent="0.35">
@@ -21940,7 +21944,7 @@
         <v>"Set the maximum tap change per iteration in STATIC solution mode. 1 is more realistic, 16 is the default for faster solution."</v>
       </c>
       <c r="I623" s="1" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="624" spans="1:9" x14ac:dyDescent="0.35">
@@ -21967,7 +21971,7 @@
         <v>"Get the number of RegControl objects in Active Circuit."</v>
       </c>
       <c r="I624" s="1" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="625" spans="1:9" x14ac:dyDescent="0.35">
@@ -21994,7 +21998,7 @@
         <v>"Get the CT primary ampere rating (secondary is 0.2 amperes)."</v>
       </c>
       <c r="I625" s="1" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="626" spans="1:9" x14ac:dyDescent="0.35">
@@ -22021,7 +22025,7 @@
         <v>"Set the CT primary ampere rating (secondary is 0.2 amperes)."</v>
       </c>
       <c r="I626" s="1" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="627" spans="1:9" x14ac:dyDescent="0.35">
@@ -22048,7 +22052,7 @@
         <v>"Get the PT ratio for voltage control settings."</v>
       </c>
       <c r="I627" s="1" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="628" spans="1:9" x14ac:dyDescent="0.35">
@@ -22075,7 +22079,7 @@
         <v>"Set the PT ratio for voltage control settings."</v>
       </c>
       <c r="I628" s="1" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="629" spans="1:9" x14ac:dyDescent="0.35">
@@ -22102,7 +22106,7 @@
         <v>"Get the LDC R settings in Volts."</v>
       </c>
       <c r="I629" s="1" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="630" spans="1:9" x14ac:dyDescent="0.35">
@@ -22129,7 +22133,7 @@
         <v>"Set the LDC R settings in Volts."</v>
       </c>
       <c r="I630" s="1" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="631" spans="1:9" x14ac:dyDescent="0.35">
@@ -22156,7 +22160,7 @@
         <v>"Get the LDC X settings in Volts."</v>
       </c>
       <c r="I631" s="1" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="632" spans="1:9" x14ac:dyDescent="0.35">
@@ -22183,7 +22187,7 @@
         <v>"Set the LDC X settings in Volts."</v>
       </c>
       <c r="I632" s="1" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="633" spans="1:9" x14ac:dyDescent="0.35">
@@ -22210,7 +22214,7 @@
         <v>"Get the reverse LDC R settings in Volts."</v>
       </c>
       <c r="I633" s="1" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="634" spans="1:9" x14ac:dyDescent="0.35">
@@ -22237,7 +22241,7 @@
         <v>"Set the reverse LDC R settings in Volts."</v>
       </c>
       <c r="I634" s="1" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="635" spans="1:9" x14ac:dyDescent="0.35">
@@ -22264,7 +22268,7 @@
         <v>"Get the reverse LDC X settings in Volts."</v>
       </c>
       <c r="I635" s="1" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="636" spans="1:9" x14ac:dyDescent="0.35">
@@ -22291,7 +22295,7 @@
         <v>"Set the reverse LDC X settings in Volts."</v>
       </c>
       <c r="I636" s="1" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="637" spans="1:9" x14ac:dyDescent="0.35">
@@ -22318,7 +22322,7 @@
         <v>"Get the time delay [s] after arming before the first tap change. Control may reset before actually changing taps."</v>
       </c>
       <c r="I637" s="1" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="638" spans="1:9" x14ac:dyDescent="0.35">
@@ -22345,7 +22349,7 @@
         <v>"Set the time delay [s] after arming before the first tap change. Control may reset before actually changing taps."</v>
       </c>
       <c r="I638" s="1" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="639" spans="1:9" x14ac:dyDescent="0.35">
@@ -22372,7 +22376,7 @@
         <v>"Get the time delay [s] for subsequent tap changes in a set. Control may reset before actually changing taps."</v>
       </c>
       <c r="I639" s="1" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="640" spans="1:9" x14ac:dyDescent="0.35">
@@ -22399,7 +22403,7 @@
         <v>"Set the time delay [s] for subsequent tap changes in a set. Control may reset before actually changing taps."</v>
       </c>
       <c r="I640" s="1" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="641" spans="1:9" x14ac:dyDescent="0.35">
@@ -22426,7 +22430,7 @@
         <v>"Get the first house voltage limit on PT secondary base. Setting to 0 disables this function."</v>
       </c>
       <c r="I641" s="1" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="642" spans="1:9" x14ac:dyDescent="0.35">
@@ -22453,7 +22457,7 @@
         <v>"Set the first house voltage limit on PT secondary base. Setting to 0 disables this function."</v>
       </c>
       <c r="I642" s="1" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="643" spans="1:9" x14ac:dyDescent="0.35">
@@ -22476,11 +22480,11 @@
         <v>710</v>
       </c>
       <c r="G643" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="G643:G706" si="10">""""&amp;TRIM(I643)&amp;""""</f>
         <v>"Get the regulation bandwidth in forward direction, centered on Vreg."</v>
       </c>
       <c r="I643" s="1" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="644" spans="1:9" x14ac:dyDescent="0.35">
@@ -22503,11 +22507,11 @@
         <v>710</v>
       </c>
       <c r="G644" s="1" t="str">
-        <f t="shared" ref="G644:G707" si="10">""""&amp;TRIM(I644)&amp;""""</f>
+        <f t="shared" si="10"/>
         <v>"Set the regulation bandwidth in forward direction, centered on Vreg."</v>
       </c>
       <c r="I644" s="1" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="645" spans="1:9" x14ac:dyDescent="0.35">
@@ -22534,7 +22538,7 @@
         <v>"Get the target voltage in the forward direction, on PT secondary base."</v>
       </c>
       <c r="I645" s="1" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="646" spans="1:9" x14ac:dyDescent="0.35">
@@ -22561,7 +22565,7 @@
         <v>"Set the target voltage in the forward direction, on PT secondary base."</v>
       </c>
       <c r="I646" s="1" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="647" spans="1:9" x14ac:dyDescent="0.35">
@@ -22588,7 +22592,7 @@
         <v>"Get the bandwidth in reverse direction, centered on reverse Vreg."</v>
       </c>
       <c r="I647" s="1" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="648" spans="1:9" x14ac:dyDescent="0.35">
@@ -22615,7 +22619,7 @@
         <v>"Set the bandwidth in reverse direction, centered on reverse Vreg."</v>
       </c>
       <c r="I648" s="1" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="649" spans="1:9" x14ac:dyDescent="0.35">
@@ -22642,7 +22646,7 @@
         <v>"Get the target voltage in the reverse direction, on PT secondary base."</v>
       </c>
       <c r="I649" s="1" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="650" spans="1:9" x14ac:dyDescent="0.35">
@@ -22669,7 +22673,7 @@
         <v>"Set the target voltage in the reverse direction, on PT secondary base."</v>
       </c>
       <c r="I650" s="1" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="651" spans="1:9" x14ac:dyDescent="0.35">
@@ -22696,7 +22700,7 @@
         <v>"Get the active RegControl name."</v>
       </c>
       <c r="I651" s="1" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="652" spans="1:9" x14ac:dyDescent="0.35">
@@ -22723,7 +22727,7 @@
         <v>"Set the active RegControl name."</v>
       </c>
       <c r="I652" s="1" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="653" spans="1:9" x14ac:dyDescent="0.35">
@@ -22750,7 +22754,7 @@
         <v>"Get the name of the remote regulated bus, in lieu of LDC settings."</v>
       </c>
       <c r="I653" s="1" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="654" spans="1:9" x14ac:dyDescent="0.35">
@@ -22777,7 +22781,7 @@
         <v>"Set the name of the remote regulated bus, in lieu of LDC settings."</v>
       </c>
       <c r="I654" s="1" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="655" spans="1:9" x14ac:dyDescent="0.35">
@@ -22804,7 +22808,7 @@
         <v>"Get the name of the transformer this regulator controls."</v>
       </c>
       <c r="I655" s="1" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="656" spans="1:9" x14ac:dyDescent="0.35">
@@ -22831,7 +22835,7 @@
         <v>"Set the name of the transformer this regulator controls."</v>
       </c>
       <c r="I656" s="1" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="657" spans="1:9" x14ac:dyDescent="0.35">
@@ -22858,7 +22862,7 @@
         <v>"Get a vector of strings containing all RegControl names."</v>
       </c>
       <c r="I657" s="1" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="658" spans="1:9" x14ac:dyDescent="0.35">
@@ -22885,7 +22889,7 @@
         <v>"Get number of Relays in active circuit."</v>
       </c>
       <c r="I658" s="1" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="659" spans="1:9" x14ac:dyDescent="0.35">
@@ -22912,7 +22916,7 @@
         <v>"Set first relay active. If none, returns 0."</v>
       </c>
       <c r="I659" s="1" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="660" spans="1:9" x14ac:dyDescent="0.35">
@@ -22939,7 +22943,7 @@
         <v>"Set next relay active. If none, returns 0."</v>
       </c>
       <c r="I660" s="1" t="s">
-        <v>1260</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="661" spans="1:9" x14ac:dyDescent="0.35">
@@ -22966,7 +22970,7 @@
         <v>"Get the number of terminal of monitored element that this relay is monitoring."</v>
       </c>
       <c r="I661" s="1" t="s">
-        <v>1261</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="662" spans="1:9" x14ac:dyDescent="0.35">
@@ -22993,7 +22997,7 @@
         <v>"Set the number of terminal of monitored element that this relay is monitoring."</v>
       </c>
       <c r="I662" s="1" t="s">
-        <v>1262</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="663" spans="1:9" x14ac:dyDescent="0.35">
@@ -23020,7 +23024,7 @@
         <v>"Get the number of terminal of the switched object that will be opened when the relay trips."</v>
       </c>
       <c r="I663" s="1" t="s">
-        <v>1263</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="664" spans="1:9" x14ac:dyDescent="0.35">
@@ -23047,7 +23051,7 @@
         <v>"Set the number of terminal of the switched object that will be opened when the relay trips."</v>
       </c>
       <c r="I664" s="1" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="665" spans="1:9" x14ac:dyDescent="0.35">
@@ -23074,7 +23078,7 @@
         <v>"Get the active relay by index into the Relay list. 1..Count."</v>
       </c>
       <c r="I665" s="1" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="666" spans="1:9" x14ac:dyDescent="0.35">
@@ -23101,7 +23105,7 @@
         <v>"Set the active relay by index into the Relay list. 1..Count."</v>
       </c>
       <c r="I666" s="1" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="667" spans="1:9" x14ac:dyDescent="0.35">
@@ -23128,7 +23132,7 @@
         <v>"Get the name of the active Relay."</v>
       </c>
       <c r="I667" s="1" t="s">
-        <v>1267</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="668" spans="1:9" x14ac:dyDescent="0.35">
@@ -23155,7 +23159,7 @@
         <v>"Set the name of the active Relay."</v>
       </c>
       <c r="I668" s="1" t="s">
-        <v>1268</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="669" spans="1:9" x14ac:dyDescent="0.35">
@@ -23182,7 +23186,7 @@
         <v>"Get the full name of the object this relay is monitoring."</v>
       </c>
       <c r="I669" s="1" t="s">
-        <v>1269</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="670" spans="1:9" x14ac:dyDescent="0.35">
@@ -23209,7 +23213,7 @@
         <v>"Set the full name of the object this relay is monitoring."</v>
       </c>
       <c r="I670" s="1" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="671" spans="1:9" x14ac:dyDescent="0.35">
@@ -23236,7 +23240,7 @@
         <v>"Get the full name of element that will switched when relay trips."</v>
       </c>
       <c r="I671" s="1" t="s">
-        <v>1271</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="672" spans="1:9" x14ac:dyDescent="0.35">
@@ -23263,7 +23267,7 @@
         <v>"Set the full name of element that will switched when relay trips."</v>
       </c>
       <c r="I672" s="1" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="673" spans="1:9" x14ac:dyDescent="0.35">
@@ -23290,7 +23294,7 @@
         <v>"Get a vector of strings containing names of all relay elements."</v>
       </c>
       <c r="I673" s="1" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="674" spans="1:9" x14ac:dyDescent="0.35">
@@ -23317,7 +23321,7 @@
         <v>"Get number of sensors in active circuit."</v>
       </c>
       <c r="I674" s="1" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="675" spans="1:9" x14ac:dyDescent="0.35">
@@ -23344,7 +23348,7 @@
         <v>"Set the first sensor active. Returns 0 if none."</v>
       </c>
       <c r="I675" s="1" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="676" spans="1:9" x14ac:dyDescent="0.35">
@@ -23371,7 +23375,7 @@
         <v>"Set the next sensor active. Returns 0 if none"</v>
       </c>
       <c r="I676" s="1" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="677" spans="1:9" x14ac:dyDescent="0.35">
@@ -23398,7 +23402,7 @@
         <v>"Returns 1 if the sensor is connected in delta; otherwise, returns 0."</v>
       </c>
       <c r="I677" s="1" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="678" spans="1:9" x14ac:dyDescent="0.35">
@@ -23425,7 +23429,7 @@
         <v>"Allows to set 1 if the sensor is connected in delta; otherwise, set 0 (argument)."</v>
       </c>
       <c r="I678" s="1" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="679" spans="1:9" x14ac:dyDescent="0.35">
@@ -23452,7 +23456,7 @@
         <v>"Returns 1 if voltage measurements are 1-3, 3-2, 2-1; otherwise 0."</v>
       </c>
       <c r="I679" s="1" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="680" spans="1:9" x14ac:dyDescent="0.35">
@@ -23479,7 +23483,7 @@
         <v>"Allows to set 1 if voltage measurements are 1-3, 3-2, 2-1; otherwise 0."</v>
       </c>
       <c r="I680" s="1" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="681" spans="1:9" x14ac:dyDescent="0.35">
@@ -23506,7 +23510,7 @@
         <v>"Get the number of the measured terminal in the measured element."</v>
       </c>
       <c r="I681" s="1" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="682" spans="1:9" x14ac:dyDescent="0.35">
@@ -23533,7 +23537,7 @@
         <v>"Set the number of the measured terminal in the measured element."</v>
       </c>
       <c r="I682" s="1" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="683" spans="1:9" x14ac:dyDescent="0.35">
@@ -23560,7 +23564,7 @@
         <v>"Clears the active sensor."</v>
       </c>
       <c r="I683" s="1" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="684" spans="1:9" x14ac:dyDescent="0.35">
@@ -23587,7 +23591,7 @@
         <v>"Clears all sensors in the active circuit."</v>
       </c>
       <c r="I684" s="1" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="685" spans="1:9" x14ac:dyDescent="0.35">
@@ -23614,7 +23618,7 @@
         <v>"Get the assumed percent error in the Sensor measurement. Default is 1."</v>
       </c>
       <c r="I685" s="1" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="686" spans="1:9" x14ac:dyDescent="0.35">
@@ -23641,7 +23645,7 @@
         <v>"Set the assumed percent error in the Sensor measurement. Default is 1."</v>
       </c>
       <c r="I686" s="1" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="687" spans="1:9" x14ac:dyDescent="0.35">
@@ -23668,7 +23672,7 @@
         <v>"Get the weighting factor for this sensor measurement with respect to the other sensors. Default is 1."</v>
       </c>
       <c r="I687" s="1" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="688" spans="1:9" x14ac:dyDescent="0.35">
@@ -23695,7 +23699,7 @@
         <v>"Set the weighting factor for this sensor measurement with respect to the other sensors. Default is 1."</v>
       </c>
       <c r="I688" s="1" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="689" spans="1:9" x14ac:dyDescent="0.35">
@@ -23722,7 +23726,7 @@
         <v>"Get the voltage base for the sensor measurements. LL for 2 and 3 - phase sensors, LN for 1-phase sensors."</v>
       </c>
       <c r="I689" s="1" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="690" spans="1:9" x14ac:dyDescent="0.35">
@@ -23749,7 +23753,7 @@
         <v>"Set the voltage base for the sensor measurements. LL for 2 and 3 - phase sensors, LN for 1-phase sensors."</v>
       </c>
       <c r="I690" s="1" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="691" spans="1:9" x14ac:dyDescent="0.35">
@@ -23776,7 +23780,7 @@
         <v>"Get the name of the active sensor object."</v>
       </c>
       <c r="I691" s="1" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="692" spans="1:9" x14ac:dyDescent="0.35">
@@ -23803,7 +23807,7 @@
         <v>"Set the name of the active sensor object."</v>
       </c>
       <c r="I692" s="1" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="693" spans="1:9" x14ac:dyDescent="0.35">
@@ -23830,7 +23834,7 @@
         <v>"Get the full name of the measured element."</v>
       </c>
       <c r="I693" s="1" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="694" spans="1:9" x14ac:dyDescent="0.35">
@@ -23857,7 +23861,7 @@
         <v>"Set the full name of the measured element."</v>
       </c>
       <c r="I694" s="1" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="695" spans="1:9" x14ac:dyDescent="0.35">
@@ -23880,11 +23884,11 @@
         <v>119</v>
       </c>
       <c r="G695" s="1" t="str">
-        <f>""""&amp;TRIM(I696)&amp;""""</f>
-        <v>"Get an array of doubles for the line current measurements; don't use with KWS and KVARS."</v>
+        <f t="shared" si="10"/>
+        <v>"Returns a vector of sensor names."</v>
       </c>
       <c r="I695" s="1" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="696" spans="1:9" x14ac:dyDescent="0.35">
@@ -23907,11 +23911,11 @@
         <v>325</v>
       </c>
       <c r="G696" s="1" t="str">
-        <f>""""&amp;TRIM(I697)&amp;""""</f>
-        <v>"Set an array of doubles for the line current measurements; don't use with KWS and KVARS."</v>
+        <f t="shared" si="10"/>
+        <v>"Get an array of doubles for the line current measurements; don't use with KWS and KVARS."</v>
       </c>
       <c r="I696" s="1" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="697" spans="1:9" x14ac:dyDescent="0.35">
@@ -23934,11 +23938,11 @@
         <v>325</v>
       </c>
       <c r="G697" s="1" t="str">
-        <f>""""&amp;TRIM(I698)&amp;""""</f>
-        <v>"Get an array of doubles for Q measurements; overwrites currents with a new estimate using KWS."</v>
+        <f t="shared" si="10"/>
+        <v>"Set an array of doubles for the line current measurements; don't use with KWS and KVARS."</v>
       </c>
       <c r="I697" s="1" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="698" spans="1:9" x14ac:dyDescent="0.35">
@@ -23961,11 +23965,11 @@
         <v>149</v>
       </c>
       <c r="G698" s="1" t="str">
-        <f>""""&amp;TRIM(I699)&amp;""""</f>
-        <v>"Set an array of doubles for Q measurements; overwrites currents with a new estimate using KWS."</v>
+        <f t="shared" si="10"/>
+        <v>"Get an array of doubles for Q measurements; overwrites currents with a new estimate using KWS."</v>
       </c>
       <c r="I698" s="1" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="699" spans="1:9" x14ac:dyDescent="0.35">
@@ -23988,11 +23992,11 @@
         <v>149</v>
       </c>
       <c r="G699" s="1" t="str">
-        <f>""""&amp;TRIM(I700)&amp;""""</f>
-        <v>"Get an array of doubles for P measurements; overwrites currents with a new estimate using KVARS."</v>
+        <f t="shared" si="10"/>
+        <v>"Set an array of doubles for Q measurements; overwrites currents with a new estimate using KWS."</v>
       </c>
       <c r="I699" s="1" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="700" spans="1:9" x14ac:dyDescent="0.35">
@@ -24015,11 +24019,11 @@
         <v>150</v>
       </c>
       <c r="G700" s="1" t="str">
-        <f>""""&amp;TRIM(I701)&amp;""""</f>
-        <v>"Set an array of doubles for P measurements; overwrites currents with a new estimate using KVARS."</v>
+        <f t="shared" si="10"/>
+        <v>"Get an array of doubles for P measurements; overwrites currents with a new estimate using KVARS."</v>
       </c>
       <c r="I700" s="1" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="701" spans="1:9" x14ac:dyDescent="0.35">
@@ -24041,12 +24045,12 @@
       <c r="F701" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G701" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G701" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>"Set an array of doubles for P measurements; overwrites currents with a new estimate using KVARS."</v>
       </c>
       <c r="I701" s="1" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="702" spans="1:9" x14ac:dyDescent="0.35">
@@ -24073,7 +24077,7 @@
         <v>"Get if OpenDSS allows duplicate names of objects: {1 allow, 0 not allow}."</v>
       </c>
       <c r="I702" s="1" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="703" spans="1:9" x14ac:dyDescent="0.35">
@@ -24100,7 +24104,7 @@
         <v>"Set if OpenDSS allows duplicate names of objects: {1 allow, 0 not allow}."</v>
       </c>
       <c r="I703" s="1" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="704" spans="1:9" x14ac:dyDescent="0.35">
@@ -24127,7 +24131,7 @@
         <v>"Get the status of Lock zones on energy meters to prevent rebuilding if a circuit change occurs: {1= true, 0= False}."</v>
       </c>
       <c r="I704" s="1" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="705" spans="1:9" x14ac:dyDescent="0.35">
@@ -24154,7 +24158,7 @@
         <v>"Set the status of Lock zones on energy meters to prevent rebuilding if a circuit change occurs: {1= true, 0= False}."</v>
       </c>
       <c r="I705" s="1" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="706" spans="1:9" x14ac:dyDescent="0.35">
@@ -24181,7 +24185,7 @@
         <v>"Get {dssMultiphase* | dssPositiveSeq} Indicate if the circuit model is positive sequence."</v>
       </c>
       <c r="I706" s="1" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="707" spans="1:9" x14ac:dyDescent="0.35">
@@ -24204,11 +24208,11 @@
         <v>732</v>
       </c>
       <c r="G707" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="G707:G770" si="11">""""&amp;TRIM(I707)&amp;""""</f>
         <v>"Set {dssMultiphase* | dssPositiveSeq} Indicate if the circuit model is positive sequence."</v>
       </c>
       <c r="I707" s="1" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="708" spans="1:9" x14ac:dyDescent="0.35">
@@ -24231,11 +24235,11 @@
         <v>733</v>
       </c>
       <c r="G708" s="1" t="str">
-        <f t="shared" ref="G708:G734" si="11">""""&amp;TRIM(I708)&amp;""""</f>
+        <f t="shared" si="11"/>
         <v>"Get {True (1) | False (0)} value of trapezoidal integration flag in Energy Meters."</v>
       </c>
       <c r="I708" s="1" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="709" spans="1:9" x14ac:dyDescent="0.35">
@@ -24262,7 +24266,7 @@
         <v>"Set {True (1) | False (0)} value of trapezoidal integration flag in Energy Meters."</v>
       </c>
       <c r="I709" s="1" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="710" spans="1:9" x14ac:dyDescent="0.35">
@@ -24289,7 +24293,7 @@
         <v>"Set all load allocation factors for all loads defined by XFKVA property to this value."</v>
       </c>
       <c r="I710" s="1" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="711" spans="1:9" x14ac:dyDescent="0.35">
@@ -24316,7 +24320,7 @@
         <v>"Get the per unit minimum voltage for Normal conditions."</v>
       </c>
       <c r="I711" s="1" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="712" spans="1:9" x14ac:dyDescent="0.35">
@@ -24343,7 +24347,7 @@
         <v>"Set the per unit minimum voltage for Normal conditions."</v>
       </c>
       <c r="I712" s="1" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="713" spans="1:9" x14ac:dyDescent="0.35">
@@ -24370,7 +24374,7 @@
         <v>"Get the per unit maximum voltage for Normal conditions."</v>
       </c>
       <c r="I713" s="1" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="714" spans="1:9" x14ac:dyDescent="0.35">
@@ -24397,7 +24401,7 @@
         <v>"Set the per unit maximum voltage for Normal conditions."</v>
       </c>
       <c r="I714" s="1" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="715" spans="1:9" x14ac:dyDescent="0.35">
@@ -24424,7 +24428,7 @@
         <v>"Get the per unit minimum voltage for Emergency conditions."</v>
       </c>
       <c r="I715" s="1" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="716" spans="1:9" x14ac:dyDescent="0.35">
@@ -24451,7 +24455,7 @@
         <v>"Set the per unit minimum voltage for Emergency conditions."</v>
       </c>
       <c r="I716" s="1" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="717" spans="1:9" x14ac:dyDescent="0.35">
@@ -24478,7 +24482,7 @@
         <v>"Get the per unit maximum voltage for Emergency conditions."</v>
       </c>
       <c r="I717" s="1" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="718" spans="1:9" x14ac:dyDescent="0.35">
@@ -24505,7 +24509,7 @@
         <v>"Set the per unit maximum voltage for Emergency conditions."</v>
       </c>
       <c r="I718" s="1" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="719" spans="1:9" x14ac:dyDescent="0.35">
@@ -24532,7 +24536,7 @@
         <v>"Get the weighting factor applied to UE register values."</v>
       </c>
       <c r="I719" s="1" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="720" spans="1:9" x14ac:dyDescent="0.35">
@@ -24559,7 +24563,7 @@
         <v>"Set the weighting factor applied to UE register values."</v>
       </c>
       <c r="I720" s="1" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="721" spans="1:9" x14ac:dyDescent="0.35">
@@ -24586,7 +24590,7 @@
         <v>"Get the weighting factor applied to Loss register values."</v>
       </c>
       <c r="I721" s="1" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="722" spans="1:9" x14ac:dyDescent="0.35">
@@ -24613,7 +24617,7 @@
         <v>"Set the weighting factor applied to Loss register values."</v>
       </c>
       <c r="I722" s="1" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="723" spans="1:9" x14ac:dyDescent="0.35">
@@ -24640,7 +24644,7 @@
         <v>"Get the price signal for the circuit."</v>
       </c>
       <c r="I723" s="1" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="724" spans="1:9" x14ac:dyDescent="0.35">
@@ -24667,7 +24671,7 @@
         <v>"Set the price signal for the circuit."</v>
       </c>
       <c r="I724" s="1" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="725" spans="1:9" x14ac:dyDescent="0.35">
@@ -24694,7 +24698,7 @@
         <v>"Get the list of Buses or (File=xxxxx) syntax for the AutoAdd solution mode."</v>
       </c>
       <c r="I725" s="1" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="726" spans="1:9" x14ac:dyDescent="0.35">
@@ -24721,7 +24725,7 @@
         <v>"Set the list of Buses or (File=xxxxx) syntax for the AutoAdd solution mode."</v>
       </c>
       <c r="I726" s="1" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="727" spans="1:9" x14ac:dyDescent="0.35">
@@ -24748,7 +24752,7 @@
         <v>"Get the name of LoadShape object that serves as the source of price signal data for yearly simulations, etc."</v>
       </c>
       <c r="I727" s="1" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="728" spans="1:9" x14ac:dyDescent="0.35">
@@ -24775,7 +24779,7 @@
         <v>"Set the name of LoadShape object that serves as the source of price signal data for yearly simulations, etc."</v>
       </c>
       <c r="I728" s="1" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="729" spans="1:9" x14ac:dyDescent="0.35">
@@ -24802,7 +24806,7 @@
         <v>"Get the array of Integers defining Energy Meter registers to use for computing UE."</v>
       </c>
       <c r="I729" s="1" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="730" spans="1:9" x14ac:dyDescent="0.35">
@@ -24829,7 +24833,7 @@
         <v>"Set the array of Integers defining Energy Meter registers to use for computing UE."</v>
       </c>
       <c r="I730" s="1" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="731" spans="1:9" x14ac:dyDescent="0.35">
@@ -24856,7 +24860,7 @@
         <v>"Get the array of Integers defining Energy Meter registers to use for computing Losses."</v>
       </c>
       <c r="I731" s="1" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="732" spans="1:9" x14ac:dyDescent="0.35">
@@ -24883,7 +24887,7 @@
         <v>"Set the array of Integers defining Energy Meter registers to use for computing Losses."</v>
       </c>
       <c r="I732" s="1" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="733" spans="1:9" x14ac:dyDescent="0.35">
@@ -24910,7 +24914,7 @@
         <v>"Get the array of doubles defining the legal voltage bases in kV L-L."</v>
       </c>
       <c r="I733" s="1" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="734" spans="1:9" x14ac:dyDescent="0.35">
@@ -24937,7 +24941,7 @@
         <v>"Set the array of doubles defining the legal voltage bases in kV L-L."</v>
       </c>
       <c r="I734" s="1" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="735" spans="1:9" x14ac:dyDescent="0.35">
@@ -24959,12 +24963,12 @@
       <c r="F735" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="G735" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G735" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>"Executes the solution for the present solution mode. Returns 0."</v>
       </c>
       <c r="I735" s="1" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="736" spans="1:9" x14ac:dyDescent="0.35">
@@ -24986,12 +24990,12 @@
       <c r="F736" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G736" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G736" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>"The present solution mode (See DSS help)."</v>
       </c>
       <c r="I736" s="1" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="737" spans="1:9" x14ac:dyDescent="0.35">
@@ -25013,12 +25017,12 @@
       <c r="F737" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G737" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G737" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>"Modifies the present solution mode (See DSS help)."</v>
       </c>
       <c r="I737" s="1" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="738" spans="1:9" x14ac:dyDescent="0.35">
@@ -25040,12 +25044,12 @@
       <c r="F738" s="1" t="s">
         <v>753</v>
       </c>
-      <c r="G738" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G738" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>"The present hour (See DSS help)."</v>
       </c>
       <c r="I738" s="1" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="739" spans="1:9" x14ac:dyDescent="0.35">
@@ -25067,12 +25071,12 @@
       <c r="F739" s="1" t="s">
         <v>753</v>
       </c>
-      <c r="G739" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G739" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>"Modifies the present hour (See DSS help)."</v>
       </c>
       <c r="I739" s="1" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="740" spans="1:9" x14ac:dyDescent="0.35">
@@ -25094,12 +25098,12 @@
       <c r="F740" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="G740" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G740" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>"The present Year (See DSS help)."</v>
       </c>
       <c r="I740" s="1" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="741" spans="1:9" x14ac:dyDescent="0.35">
@@ -25121,12 +25125,12 @@
       <c r="F741" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="G741" s="1" t="e">
-        <f>""""&amp;TRIM(#REF!)&amp;""""</f>
-        <v>#REF!</v>
+      <c r="G741" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>"Modifies the present Year (See DSS help)."</v>
       </c>
       <c r="I741" s="1" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="742" spans="1:9" x14ac:dyDescent="0.35">
@@ -25149,11 +25153,11 @@
         <v>755</v>
       </c>
       <c r="G742" s="1" t="str">
-        <f>""""&amp;TRIM(I735)&amp;""""</f>
-        <v>"Executes the solution for the present solution mode. Returns 0."</v>
+        <f t="shared" si="11"/>
+        <v>"Return the number of iterations taken for the last solution."</v>
       </c>
       <c r="I742" s="1" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="743" spans="1:9" x14ac:dyDescent="0.35">
@@ -25176,11 +25180,11 @@
         <v>756</v>
       </c>
       <c r="G743" s="1" t="str">
-        <f>""""&amp;TRIM(I736)&amp;""""</f>
-        <v>"The present solution mode (See DSS help)."</v>
+        <f t="shared" si="11"/>
+        <v>"The Maximum number of iterations used to solve the circuit."</v>
       </c>
       <c r="I743" s="1" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="744" spans="1:9" x14ac:dyDescent="0.35">
@@ -25203,11 +25207,11 @@
         <v>756</v>
       </c>
       <c r="G744" s="1" t="str">
-        <f>""""&amp;TRIM(I737)&amp;""""</f>
-        <v>"Modifies the present solution mode (See DSS help)."</v>
+        <f t="shared" si="11"/>
+        <v>"Modifies the Maximum number of iterations used to solve the circuit."</v>
       </c>
       <c r="I744" s="1" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="745" spans="1:9" x14ac:dyDescent="0.35">
@@ -25230,11 +25234,11 @@
         <v>757</v>
       </c>
       <c r="G745" s="1" t="str">
-        <f>""""&amp;TRIM(I738)&amp;""""</f>
-        <v>"The present hour (See DSS help)."</v>
+        <f t="shared" si="11"/>
+        <v>"The number of solutions to perform for MonteCarlo and time series simulations."</v>
       </c>
       <c r="I745" s="1" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="746" spans="1:9" x14ac:dyDescent="0.35">
@@ -25257,11 +25261,11 @@
         <v>757</v>
       </c>
       <c r="G746" s="1" t="str">
-        <f>""""&amp;TRIM(I739)&amp;""""</f>
-        <v>"Modifies the present hour (See DSS help)."</v>
+        <f t="shared" si="11"/>
+        <v>"Modifies the number of solutions to perform for MonteCarlo and time series simulations."</v>
       </c>
       <c r="I746" s="1" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="747" spans="1:9" x14ac:dyDescent="0.35">
@@ -25284,11 +25288,11 @@
         <v>758</v>
       </c>
       <c r="G747" s="1" t="str">
-        <f>""""&amp;TRIM(I740)&amp;""""</f>
-        <v>"The present Year (See DSS help)."</v>
+        <f t="shared" si="11"/>
+        <v>"The randomization mode for random variables "Gaussian" o "Uniform"."</v>
       </c>
       <c r="I747" s="1" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="748" spans="1:9" x14ac:dyDescent="0.35">
@@ -25311,11 +25315,11 @@
         <v>758</v>
       </c>
       <c r="G748" s="1" t="str">
-        <f>""""&amp;TRIM(I741)&amp;""""</f>
-        <v>"Modifies the present Year (See DSS help)."</v>
+        <f t="shared" si="11"/>
+        <v>"Modifies the randomization mode for random variables "Gaussian" o "Uniform"."</v>
       </c>
       <c r="I748" s="1" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="749" spans="1:9" x14ac:dyDescent="0.35">
@@ -25338,11 +25342,11 @@
         <v>759</v>
       </c>
       <c r="G749" s="1" t="str">
-        <f>""""&amp;TRIM(I742)&amp;""""</f>
-        <v>"Return the number of iterations taken for the last solution."</v>
+        <f t="shared" si="11"/>
+        <v>"The Load Model: {dssPowerFlow (default)|dssAdmittance}."</v>
       </c>
       <c r="I749" s="1" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="750" spans="1:9" x14ac:dyDescent="0.35">
@@ -25365,11 +25369,11 @@
         <v>759</v>
       </c>
       <c r="G750" s="1" t="str">
-        <f>""""&amp;TRIM(I743)&amp;""""</f>
-        <v>"The Maximum number of iterations used to solve the circuit."</v>
+        <f t="shared" si="11"/>
+        <v>"Modifies the Load Model: {dssPowerFlow (default)|dssAdmittance}."</v>
       </c>
       <c r="I750" s="1" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="751" spans="1:9" x14ac:dyDescent="0.35">
@@ -25392,11 +25396,11 @@
         <v>760</v>
       </c>
       <c r="G751" s="1" t="str">
-        <f>""""&amp;TRIM(I744)&amp;""""</f>
-        <v>"Modifies the Maximum number of iterations used to solve the circuit."</v>
+        <f t="shared" si="11"/>
+        <v>"The type of device to add in AutoAdd Mode: {dssGen (default)|dssCap}."</v>
       </c>
       <c r="I751" s="1" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="752" spans="1:9" x14ac:dyDescent="0.35">
@@ -25419,11 +25423,11 @@
         <v>760</v>
       </c>
       <c r="G752" s="1" t="str">
-        <f>""""&amp;TRIM(I745)&amp;""""</f>
-        <v>"The number of solutions to perform for MonteCarlo and time series simulations."</v>
+        <f t="shared" si="11"/>
+        <v>"Modifies the type of device to add in AutoAdd Mode: {dssGen (default)|dssCap}."</v>
       </c>
       <c r="I752" s="1" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="753" spans="1:9" x14ac:dyDescent="0.35">
@@ -25446,11 +25450,11 @@
         <v>761</v>
       </c>
       <c r="G753" s="1" t="str">
-        <f>""""&amp;TRIM(I746)&amp;""""</f>
-        <v>"Modifies the number of solutions to perform for MonteCarlo and time series simulations."</v>
+        <f t="shared" si="11"/>
+        <v>"The base solution algorithm: {dssNormalSolve | dssNewtonSolve}."</v>
       </c>
       <c r="I753" s="1" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="754" spans="1:9" x14ac:dyDescent="0.35">
@@ -25473,11 +25477,11 @@
         <v>761</v>
       </c>
       <c r="G754" s="1" t="str">
-        <f>""""&amp;TRIM(I747)&amp;""""</f>
-        <v>"The randomization mode for random variables "Gaussian" o "Uniform"."</v>
+        <f t="shared" si="11"/>
+        <v>"Modifies the base solution algorithm: {dssNormalSolve | dssNewtonSolve}."</v>
       </c>
       <c r="I754" s="1" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="755" spans="1:9" x14ac:dyDescent="0.35">
@@ -25500,11 +25504,11 @@
         <v>762</v>
       </c>
       <c r="G755" s="1" t="str">
-        <f>""""&amp;TRIM(I748)&amp;""""</f>
-        <v>"Modifies the randomization mode for random variables "Gaussian" o "Uniform"."</v>
+        <f t="shared" si="11"/>
+        <v>"The mode for control devices: {dssStatic (default) | dssEvent | dssTime}."</v>
       </c>
       <c r="I755" s="1" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="756" spans="1:9" x14ac:dyDescent="0.35">
@@ -25527,11 +25531,11 @@
         <v>762</v>
       </c>
       <c r="G756" s="1" t="str">
-        <f>""""&amp;TRIM(I749)&amp;""""</f>
-        <v>"The Load Model: {dssPowerFlow (default)|dssAdmittance}."</v>
+        <f t="shared" si="11"/>
+        <v>"Modifies the mode for control devices: {dssStatic (default) | dssEvent | dssTime}."</v>
       </c>
       <c r="I756" s="1" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="757" spans="1:9" x14ac:dyDescent="0.35">
@@ -25554,11 +25558,11 @@
         <v>763</v>
       </c>
       <c r="G757" s="1" t="str">
-        <f>""""&amp;TRIM(I750)&amp;""""</f>
-        <v>"Modifies the Load Model: {dssPowerFlow (default)|dssAdmittance}."</v>
+        <f t="shared" si="11"/>
+        <v>"The current value of the control iteration counter."</v>
       </c>
       <c r="I757" s="1" t="s">
-        <v>1357</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="758" spans="1:9" x14ac:dyDescent="0.35">
@@ -25581,11 +25585,11 @@
         <v>763</v>
       </c>
       <c r="G758" s="1" t="str">
-        <f>""""&amp;TRIM(I751)&amp;""""</f>
-        <v>"The type of device to add in AutoAdd Mode: {dssGen (default)|dssCap}."</v>
+        <f t="shared" si="11"/>
+        <v>"Modifies the current value of the control iteration counter."</v>
       </c>
       <c r="I758" s="1" t="s">
-        <v>1358</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="759" spans="1:9" x14ac:dyDescent="0.35">
@@ -25608,11 +25612,11 @@
         <v>764</v>
       </c>
       <c r="G759" s="1" t="str">
-        <f>""""&amp;TRIM(I752)&amp;""""</f>
-        <v>"Modifies the type of device to add in AutoAdd Mode: {dssGen (default)|dssCap}."</v>
+        <f t="shared" si="11"/>
+        <v>"The maximum allowable control iterations."</v>
       </c>
       <c r="I759" s="1" t="s">
-        <v>1359</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="760" spans="1:9" x14ac:dyDescent="0.35">
@@ -25635,11 +25639,11 @@
         <v>764</v>
       </c>
       <c r="G760" s="1" t="str">
-        <f>""""&amp;TRIM(I753)&amp;""""</f>
-        <v>"The base solution algorithm: {dssNormalSolve | dssNewtonSolve}."</v>
+        <f t="shared" si="11"/>
+        <v>"Modifies the maximum allowable control iterations."</v>
       </c>
       <c r="I760" s="1" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="761" spans="1:9" x14ac:dyDescent="0.35">
@@ -25662,11 +25666,11 @@
         <v>765</v>
       </c>
       <c r="G761" s="1" t="str">
-        <f>""""&amp;TRIM(I754)&amp;""""</f>
-        <v>"Modifies the base solution algorithm: {dssNormalSolve | dssNewtonSolve}."</v>
+        <f t="shared" si="11"/>
+        <v>"Sample controls and then process the control queue for present control mode and dispatch control actions. Returns 0."</v>
       </c>
       <c r="I761" s="1" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="762" spans="1:9" x14ac:dyDescent="0.35">
@@ -25689,11 +25693,11 @@
         <v>766</v>
       </c>
       <c r="G762" s="1" t="str">
-        <f>""""&amp;TRIM(I755)&amp;""""</f>
-        <v>"The mode for control devices: {dssStatic (default) | dssEvent | dssTime}."</v>
+        <f t="shared" si="11"/>
+        <v>"Executes status check on all fault objects defined in the circuit. Returns 0."</v>
       </c>
       <c r="I762" s="1" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="763" spans="1:9" x14ac:dyDescent="0.35">
@@ -25716,11 +25720,11 @@
         <v>767</v>
       </c>
       <c r="G763" s="1" t="str">
-        <f>""""&amp;TRIM(I756)&amp;""""</f>
-        <v>"Modifies the mode for control devices: {dssStatic (default) | dssEvent | dssTime}."</v>
+        <f t="shared" si="11"/>
+        <v>"Executes a direct solution from the system Y matrix, ignoring compensation currents of loads, generators (includes Yprim only)."</v>
       </c>
       <c r="I763" s="1" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="764" spans="1:9" x14ac:dyDescent="0.35">
@@ -25743,11 +25747,11 @@
         <v>768</v>
       </c>
       <c r="G764" s="1" t="str">
-        <f>""""&amp;TRIM(I757)&amp;""""</f>
-        <v>"The current value of the control iteration counter."</v>
+        <f t="shared" si="11"/>
+        <v>"Solves using present power flow method. Iterative solution rather than direct solution."</v>
       </c>
       <c r="I764" s="1" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="765" spans="1:9" x14ac:dyDescent="0.35">
@@ -25770,11 +25774,11 @@
         <v>769</v>
       </c>
       <c r="G765" s="1" t="str">
-        <f>""""&amp;TRIM(I758)&amp;""""</f>
-        <v>"Modifies the current value of the control iteration counter."</v>
+        <f t="shared" si="11"/>
+        <v>"Is similar to SolveSnap except no control actions are checked or executed."</v>
       </c>
       <c r="I765" s="1" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="766" spans="1:9" x14ac:dyDescent="0.35">
@@ -25797,11 +25801,11 @@
         <v>770</v>
       </c>
       <c r="G766" s="1" t="str">
-        <f>""""&amp;TRIM(I759)&amp;""""</f>
-        <v>"The maximum allowable control iterations."</v>
+        <f t="shared" si="11"/>
+        <v>"Executes a power flow solution (SolveNoControl) plus executes a CheckControlActions that executes any pending control actions."</v>
       </c>
       <c r="I766" s="1" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="767" spans="1:9" x14ac:dyDescent="0.35">
@@ -25824,11 +25828,11 @@
         <v>771</v>
       </c>
       <c r="G767" s="1" t="str">
-        <f>""""&amp;TRIM(I760)&amp;""""</f>
-        <v>"Modifies the maximum allowable control iterations."</v>
+        <f t="shared" si="11"/>
+        <v>"Initializes some variables for snap shot power flow. SolveSnap does this automatically."</v>
       </c>
       <c r="I767" s="1" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="768" spans="1:9" x14ac:dyDescent="0.35">
@@ -25851,11 +25855,11 @@
         <v>772</v>
       </c>
       <c r="G768" s="1" t="str">
-        <f>""""&amp;TRIM(I761)&amp;""""</f>
-        <v>"Sample controls and then process the control queue for present control mode and dispatch control actions. Returns 0."</v>
+        <f t="shared" si="11"/>
+        <v>"Performs the normal process for sampling and executing Control Actions and Fault Status and rebuilds Y if necessary."</v>
       </c>
       <c r="I768" s="1" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="769" spans="1:9" x14ac:dyDescent="0.35">
@@ -25878,11 +25882,11 @@
         <v>773</v>
       </c>
       <c r="G769" s="1" t="str">
-        <f>""""&amp;TRIM(I762)&amp;""""</f>
-        <v>"Executes status check on all fault objects defined in the circuit. Returns 0."</v>
+        <f t="shared" si="11"/>
+        <v>"Executes a sampling of all intrinsic control devices, which push control actions into the control queue."</v>
       </c>
       <c r="I769" s="1" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="770" spans="1:9" x14ac:dyDescent="0.35">
@@ -25905,11 +25909,11 @@
         <v>774</v>
       </c>
       <c r="G770" s="1" t="str">
-        <f>""""&amp;TRIM(I763)&amp;""""</f>
-        <v>"Executes a direct solution from the system Y matrix, ignoring compensation currents of loads, generators (includes Yprim only)."</v>
+        <f t="shared" si="11"/>
+        <v>"Pops control actions off the control queue and dispatches to the proper control element."</v>
       </c>
       <c r="I770" s="1" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="771" spans="1:9" x14ac:dyDescent="0.35">
@@ -25932,11 +25936,11 @@
         <v>775</v>
       </c>
       <c r="G771" s="1" t="str">
-        <f>""""&amp;TRIM(I764)&amp;""""</f>
-        <v>"Solves using present power flow method. Iterative solution rather than direct solution."</v>
+        <f t="shared" ref="G771:G834" si="12">""""&amp;TRIM(I771)&amp;""""</f>
+        <v>"Forces building of the System Y matrix according to the argument: {1= series elements only | 2= Whole Y matrix}."</v>
       </c>
       <c r="I771" s="1" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="772" spans="1:9" x14ac:dyDescent="0.35">
@@ -25959,11 +25963,11 @@
         <v>776</v>
       </c>
       <c r="G772" s="1" t="str">
-        <f>""""&amp;TRIM(I765)&amp;""""</f>
-        <v>"Is similar to SolveSnap except no control actions are checked or executed."</v>
+        <f t="shared" si="12"/>
+        <v>"Indicates if elements of the System Y have been changed by recent activity. If changed returns 1; otherwise 0."</v>
       </c>
       <c r="I772" s="1" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="773" spans="1:9" x14ac:dyDescent="0.35">
@@ -25986,11 +25990,11 @@
         <v>777</v>
       </c>
       <c r="G773" s="1" t="str">
-        <f>""""&amp;TRIM(I766)&amp;""""</f>
-        <v>"Executes a power flow solution (SolveNoControl) plus executes a CheckControlActions that executes any pending control actions."</v>
+        <f t="shared" si="12"/>
+        <v>"Indicates whether the circuit solution converged (1 converged | 0 not converged)."</v>
       </c>
       <c r="I773" s="1" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="774" spans="1:9" x14ac:dyDescent="0.35">
@@ -26013,11 +26017,11 @@
         <v>777</v>
       </c>
       <c r="G774" s="1" t="str">
-        <f>""""&amp;TRIM(I767)&amp;""""</f>
-        <v>"Initializes some variables for snap shot power flow. SolveSnap does this automatically."</v>
+        <f t="shared" si="12"/>
+        <v>"Modifies the converged flag (1 converged | 0 not converged)."</v>
       </c>
       <c r="I774" s="1" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="775" spans="1:9" x14ac:dyDescent="0.35">
@@ -26040,11 +26044,11 @@
         <v>778</v>
       </c>
       <c r="G775" s="1" t="str">
-        <f>""""&amp;TRIM(I768)&amp;""""</f>
-        <v>"Performs the normal process for sampling and executing Control Actions and Fault Status and rebuilds Y if necessary."</v>
+        <f t="shared" si="12"/>
+        <v>"The total iterations including control iterations for most recent solution."</v>
       </c>
       <c r="I775" s="1" t="s">
-        <v>1375</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="776" spans="1:9" x14ac:dyDescent="0.35">
@@ -26067,11 +26071,11 @@
         <v>779</v>
       </c>
       <c r="G776" s="1" t="str">
-        <f>""""&amp;TRIM(I769)&amp;""""</f>
-        <v>"Executes a sampling of all intrinsic control devices, which push control actions into the control queue."</v>
+        <f t="shared" si="12"/>
+        <v>"The max number of iterations required to converge at any control iteration of the most recent solution."</v>
       </c>
       <c r="I776" s="1" t="s">
-        <v>1376</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="777" spans="1:9" x14ac:dyDescent="0.35">
@@ -26094,11 +26098,11 @@
         <v>780</v>
       </c>
       <c r="G777" s="1" t="str">
-        <f>""""&amp;TRIM(I770)&amp;""""</f>
-        <v>"Pops control actions off the control queue and dispatches to the proper control element."</v>
+        <f t="shared" si="12"/>
+        <v>"Indicates that the control actions are done: {1 done, 0 not done}."</v>
       </c>
       <c r="I777" s="1" t="s">
-        <v>1377</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="778" spans="1:9" x14ac:dyDescent="0.35">
@@ -26121,11 +26125,11 @@
         <v>780</v>
       </c>
       <c r="G778" s="1" t="str">
-        <f>""""&amp;TRIM(I771)&amp;""""</f>
-        <v>"Forces building of the System Y matrix according to the argument: {1= series elements only | 2= Whole Y matrix}."</v>
+        <f t="shared" si="12"/>
+        <v>"Modifies the flag to indicate that the control actions are done: {1 done, 0 not done}."</v>
       </c>
       <c r="I778" s="1" t="s">
-        <v>1378</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="779" spans="1:9" x14ac:dyDescent="0.35">
@@ -26148,11 +26152,11 @@
         <v>781</v>
       </c>
       <c r="G779" s="1" t="str">
-        <f>""""&amp;TRIM(I772)&amp;""""</f>
-        <v>"Indicates if elements of the System Y have been changed by recent activity. If changed returns 1; otherwise 0."</v>
+        <f t="shared" si="12"/>
+        <v>"Call cleanup, sample monitors, and increment time at end of time step."</v>
       </c>
       <c r="I779" s="1" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="780" spans="1:9" x14ac:dyDescent="0.35">
@@ -26175,11 +26179,11 @@
         <v>782</v>
       </c>
       <c r="G780" s="1" t="str">
-        <f>""""&amp;TRIM(I773)&amp;""""</f>
-        <v>"Indicates whether the circuit solution converged (1 converged | 0 not converged)."</v>
+        <f t="shared" si="12"/>
+        <v>"Update storage, invcontrol, etc., at end of time step."</v>
       </c>
       <c r="I780" s="1" t="s">
-        <v>1380</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="781" spans="1:9" x14ac:dyDescent="0.35">
@@ -26202,11 +26206,11 @@
         <v>463</v>
       </c>
       <c r="G781" s="1" t="str">
-        <f>""""&amp;TRIM(I774)&amp;""""</f>
-        <v>"Modifies the converged flag (1 converged | 0 not converged)."</v>
+        <f t="shared" si="12"/>
+        <v>"The frequency for the next solution."</v>
       </c>
       <c r="I781" s="1" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="782" spans="1:9" x14ac:dyDescent="0.35">
@@ -26229,11 +26233,11 @@
         <v>463</v>
       </c>
       <c r="G782" s="1" t="str">
-        <f>""""&amp;TRIM(I775)&amp;""""</f>
-        <v>"The total iterations including control iterations for most recent solution."</v>
+        <f t="shared" si="12"/>
+        <v>"Set the frequency for the next solution."</v>
       </c>
       <c r="I782" s="1" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="783" spans="1:9" x14ac:dyDescent="0.35">
@@ -26256,11 +26260,11 @@
         <v>786</v>
       </c>
       <c r="G783" s="1" t="str">
-        <f>""""&amp;TRIM(I776)&amp;""""</f>
-        <v>"The max number of iterations required to converge at any control iteration of the most recent solution."</v>
+        <f t="shared" si="12"/>
+        <v>"The seconds from top of the hour."</v>
       </c>
       <c r="I783" s="1" t="s">
-        <v>1383</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="784" spans="1:9" x14ac:dyDescent="0.35">
@@ -26283,11 +26287,11 @@
         <v>786</v>
       </c>
       <c r="G784" s="1" t="str">
-        <f>""""&amp;TRIM(I777)&amp;""""</f>
-        <v>"Indicates that the control actions are done: {1 done, 0 not done}."</v>
+        <f t="shared" si="12"/>
+        <v>"Set the seconds from top of the hour."</v>
       </c>
       <c r="I784" s="1" t="s">
-        <v>1384</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="785" spans="1:9" x14ac:dyDescent="0.35">
@@ -26310,11 +26314,11 @@
         <v>787</v>
       </c>
       <c r="G785" s="1" t="str">
-        <f>""""&amp;TRIM(I778)&amp;""""</f>
-        <v>"Modifies the flag to indicate that the control actions are done: {1 done, 0 not done}."</v>
+        <f t="shared" si="12"/>
+        <v>"The step size for the next solution."</v>
       </c>
       <c r="I785" s="1" t="s">
-        <v>1385</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="786" spans="1:9" x14ac:dyDescent="0.35">
@@ -26337,11 +26341,11 @@
         <v>787</v>
       </c>
       <c r="G786" s="1" t="str">
-        <f>""""&amp;TRIM(I779)&amp;""""</f>
-        <v>"Call cleanup, sample monitors, and increment time at end of time step."</v>
+        <f t="shared" si="12"/>
+        <v>"Set the step size for the next solution."</v>
       </c>
       <c r="I786" s="1" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="787" spans="1:9" x14ac:dyDescent="0.35">
@@ -26364,11 +26368,11 @@
         <v>788</v>
       </c>
       <c r="G787" s="1" t="str">
-        <f>""""&amp;TRIM(I780)&amp;""""</f>
-        <v>"Update storage, invcontrol, etc., at end of time step."</v>
+        <f t="shared" si="12"/>
+        <v>"The default load multiplier applied to all non-fixed loads."</v>
       </c>
       <c r="I787" s="1" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="788" spans="1:9" x14ac:dyDescent="0.35">
@@ -26391,11 +26395,11 @@
         <v>788</v>
       </c>
       <c r="G788" s="1" t="str">
-        <f t="shared" ref="G788:G835" si="12">""""&amp;TRIM(I788)&amp;""""</f>
+        <f t="shared" si="12"/>
         <v>"Set the default load multiplier applied to all non-fixed loads."</v>
       </c>
       <c r="I788" s="1" t="s">
-        <v>1388</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="789" spans="1:9" x14ac:dyDescent="0.35">
@@ -26422,7 +26426,7 @@
         <v>"The solution convergence tolerance."</v>
       </c>
       <c r="I789" s="1" t="s">
-        <v>1389</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="790" spans="1:9" x14ac:dyDescent="0.35">
@@ -26449,7 +26453,7 @@
         <v>"Set the solution convergence tolerance."</v>
       </c>
       <c r="I790" s="1" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="791" spans="1:9" x14ac:dyDescent="0.35">
@@ -26476,7 +26480,7 @@
         <v>"The percent default annual load growth rate."</v>
       </c>
       <c r="I791" s="1" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="792" spans="1:9" x14ac:dyDescent="0.35">
@@ -26503,7 +26507,7 @@
         <v>"Set the percent default annual load growth rate."</v>
       </c>
       <c r="I792" s="1" t="s">
-        <v>1392</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="793" spans="1:9" x14ac:dyDescent="0.35">
@@ -26530,7 +26534,7 @@
         <v>"The generator kW for AutoAdd mode."</v>
       </c>
       <c r="I793" s="1" t="s">
-        <v>1393</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="794" spans="1:9" x14ac:dyDescent="0.35">
@@ -26557,7 +26561,7 @@
         <v>"Set the generator kW for AutoAdd mode."</v>
       </c>
       <c r="I794" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="795" spans="1:9" x14ac:dyDescent="0.35">
@@ -26584,7 +26588,7 @@
         <v>"The pf for generators in AutoAdd mode."</v>
       </c>
       <c r="I795" s="1" t="s">
-        <v>1395</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="796" spans="1:9" x14ac:dyDescent="0.35">
@@ -26611,7 +26615,7 @@
         <v>"Set the pf for generators in AutoAdd mode."</v>
       </c>
       <c r="I796" s="1" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="797" spans="1:9" x14ac:dyDescent="0.35">
@@ -26638,7 +26642,7 @@
         <v>"The capacitor kvar for adding in AutoAdd mode."</v>
       </c>
       <c r="I797" s="1" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="798" spans="1:9" x14ac:dyDescent="0.35">
@@ -26665,7 +26669,7 @@
         <v>"Set the capacitor kvar for adding in AutoAdd mode."</v>
       </c>
       <c r="I798" s="1" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="799" spans="1:9" x14ac:dyDescent="0.35">
@@ -26692,7 +26696,7 @@
         <v>"The default multiplier applied to generators (like LoadMult)."</v>
       </c>
       <c r="I799" s="1" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="800" spans="1:9" x14ac:dyDescent="0.35">
@@ -26719,7 +26723,7 @@
         <v>"Set the default multiplier applied to generators (like LoadMult)."</v>
       </c>
       <c r="I800" s="1" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="801" spans="1:9" x14ac:dyDescent="0.35">
@@ -26746,7 +26750,7 @@
         <v>"The hour as a double, including fractional part."</v>
       </c>
       <c r="I801" s="1" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="802" spans="1:9" x14ac:dyDescent="0.35">
@@ -26773,7 +26777,7 @@
         <v>"Set the hour as a double, including fractional part."</v>
       </c>
       <c r="I802" s="1" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="803" spans="1:9" x14ac:dyDescent="0.35">
@@ -26800,7 +26804,7 @@
         <v>"Set the step size in minutes."</v>
       </c>
       <c r="I803" s="1" t="s">
-        <v>1403</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="804" spans="1:9" x14ac:dyDescent="0.35">
@@ -26827,7 +26831,7 @@
         <v>"Set the step size in Hours."</v>
       </c>
       <c r="I804" s="1" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="805" spans="1:9" x14ac:dyDescent="0.35">
@@ -26854,7 +26858,7 @@
         <v>"The ID (text) of the present solution mode."</v>
       </c>
       <c r="I805" s="1" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="806" spans="1:9" x14ac:dyDescent="0.35">
@@ -26881,7 +26885,7 @@
         <v>"The Load-Duration Curve name for LD modes."</v>
       </c>
       <c r="I806" s="1" t="s">
-        <v>1406</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="807" spans="1:9" x14ac:dyDescent="0.35">
@@ -26908,7 +26912,7 @@
         <v>"Set the Load-Duration Curve name for LD modes."</v>
       </c>
       <c r="I807" s="1" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="808" spans="1:9" x14ac:dyDescent="0.35">
@@ -26935,7 +26939,7 @@
         <v>"The default daily load shape (defaults to "Default")."</v>
       </c>
       <c r="I808" s="1" t="s">
-        <v>1408</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="809" spans="1:9" x14ac:dyDescent="0.35">
@@ -26962,7 +26966,7 @@
         <v>"Set the default daily load shape (defaults to "Default")."</v>
       </c>
       <c r="I809" s="1" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="810" spans="1:9" x14ac:dyDescent="0.35">
@@ -26989,7 +26993,7 @@
         <v>"The default yearly load shape (defaults to "Default")."</v>
       </c>
       <c r="I810" s="1" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="811" spans="1:9" x14ac:dyDescent="0.35">
@@ -27016,7 +27020,7 @@
         <v>"Set the default yearly load shape (defaults to "Default")."</v>
       </c>
       <c r="I811" s="1" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="812" spans="1:9" x14ac:dyDescent="0.35">
@@ -27043,7 +27047,7 @@
         <v>"Returns an array of strings containing the Event Log."</v>
       </c>
       <c r="I812" s="1" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="813" spans="1:9" x14ac:dyDescent="0.35">
@@ -27070,7 +27074,7 @@
         <v>"Set the first SwtControl active. Returns 0 if no more."</v>
       </c>
       <c r="I813" s="1" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="814" spans="1:9" x14ac:dyDescent="0.35">
@@ -27097,7 +27101,7 @@
         <v>"Set the next SwtControl active. Returns 0 if no more."</v>
       </c>
       <c r="I814" s="1" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="815" spans="1:9" x14ac:dyDescent="0.35">
@@ -27124,7 +27128,7 @@
         <v>"Get the open (1) or close (2) action of the switch. No effect if switch is locked. However, reset removes any lock and then closes the switch (shelf state). 0 = none action."</v>
       </c>
       <c r="I815" s="1" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="816" spans="1:9" x14ac:dyDescent="0.35">
@@ -27151,7 +27155,7 @@
         <v>"Set open (1) or close (2) the switch. No effect if switch is locked. However, reset removes any lock and then closes the switch (shelf state). 0 = none action (see manual for details)."</v>
       </c>
       <c r="I816" s="1" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="817" spans="1:9" x14ac:dyDescent="0.35">
@@ -27178,7 +27182,7 @@
         <v>"Get the lock state: {1 locked | 0 not locked}."</v>
       </c>
       <c r="I817" s="1" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="818" spans="1:9" x14ac:dyDescent="0.35">
@@ -27205,7 +27209,7 @@
         <v>"Set the lock to prevent both manual and automatic switch operation."</v>
       </c>
       <c r="I818" s="1" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="819" spans="1:9" x14ac:dyDescent="0.35">
@@ -27232,7 +27236,7 @@
         <v>"Get the terminal number where the switch is located on the SwitchedObj."</v>
       </c>
       <c r="I819" s="1" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="820" spans="1:9" x14ac:dyDescent="0.35">
@@ -27259,7 +27263,7 @@
         <v>"Set the terminal number where the switch is located on the SwitchedObj."</v>
       </c>
       <c r="I820" s="1" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="821" spans="1:9" x14ac:dyDescent="0.35">
@@ -27286,7 +27290,7 @@
         <v>"Get the total number of SwtControls in the active circuit."</v>
       </c>
       <c r="I821" s="1" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="822" spans="1:9" x14ac:dyDescent="0.35">
@@ -27313,7 +27317,7 @@
         <v>"Get the time delay [s] between arming and opening or closing the switch. Control may reset before actually operating the switch."</v>
       </c>
       <c r="I822" s="1" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="823" spans="1:9" x14ac:dyDescent="0.35">
@@ -27340,7 +27344,7 @@
         <v>"Set the time delay [s] between arming and opening or closing the switch. Control may reset before actually operating the switch."</v>
       </c>
       <c r="I823" s="1" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="824" spans="1:9" x14ac:dyDescent="0.35">
@@ -27367,7 +27371,7 @@
         <v>"Get the name of the active SwtControl."</v>
       </c>
       <c r="I824" s="1" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="825" spans="1:9" x14ac:dyDescent="0.35">
@@ -27394,7 +27398,7 @@
         <v>"Set a SwtControl active by name."</v>
       </c>
       <c r="I825" s="1" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="826" spans="1:9" x14ac:dyDescent="0.35">
@@ -27421,7 +27425,7 @@
         <v>"Get the name of the switched object by the active SwtControl."</v>
       </c>
       <c r="I826" s="1" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="827" spans="1:9" x14ac:dyDescent="0.35">
@@ -27448,7 +27452,7 @@
         <v>"Set the switched object by name."</v>
       </c>
       <c r="I827" s="1" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="828" spans="1:9" x14ac:dyDescent="0.35">
@@ -27475,7 +27479,7 @@
         <v>"Get a vector of strings with all SwtControl names in the active circuit."</v>
       </c>
       <c r="I828" s="1" t="s">
-        <v>1428</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="829" spans="1:9" x14ac:dyDescent="0.35">
@@ -27502,7 +27506,7 @@
         <v>"Get the number of loops."</v>
       </c>
       <c r="I829" s="1" t="s">
-        <v>1429</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="830" spans="1:9" x14ac:dyDescent="0.35">
@@ -27529,7 +27533,7 @@
         <v>"Get the number of isolated branches (PD elements and capacitors)."</v>
       </c>
       <c r="I830" s="1" t="s">
-        <v>1430</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="831" spans="1:9" x14ac:dyDescent="0.35">
@@ -27556,7 +27560,7 @@
         <v>"Get the number of isolated loads."</v>
       </c>
       <c r="I831" s="1" t="s">
-        <v>1431</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="832" spans="1:9" x14ac:dyDescent="0.35">
@@ -27583,7 +27587,7 @@
         <v>"Set the first branch active, returns 0 if none."</v>
       </c>
       <c r="I832" s="1" t="s">
-        <v>1432</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="833" spans="1:9" x14ac:dyDescent="0.35">
@@ -27610,7 +27614,7 @@
         <v>"Set the next branch active, returns 0 if none."</v>
       </c>
       <c r="I833" s="1" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="834" spans="1:9" x14ac:dyDescent="0.35">
@@ -27637,7 +27641,7 @@
         <v>"The index of the active Branch."</v>
       </c>
       <c r="I834" s="1" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="835" spans="1:9" x14ac:dyDescent="0.35">
@@ -27660,11 +27664,11 @@
         <v>814</v>
       </c>
       <c r="G835" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="G835:G898" si="13">""""&amp;TRIM(I835)&amp;""""</f>
         <v>"Move forward in the tree, return index of new active branch or 0 if no more."</v>
       </c>
       <c r="I835" s="1" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="836" spans="1:9" x14ac:dyDescent="0.35">
@@ -27687,11 +27691,11 @@
         <v>815</v>
       </c>
       <c r="G836" s="1" t="str">
-        <f t="shared" ref="G836:G897" si="13">""""&amp;TRIM(I836)&amp;""""</f>
+        <f t="shared" si="13"/>
         <v>"Move back toward the source, return index of new active branch or 0 if no more."</v>
       </c>
       <c r="I836" s="1" t="s">
-        <v>1436</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="837" spans="1:9" x14ac:dyDescent="0.35">
@@ -27718,7 +27722,7 @@
         <v>"Move to looped branch, return index or 0 if none."</v>
       </c>
       <c r="I837" s="1" t="s">
-        <v>1437</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="838" spans="1:9" x14ac:dyDescent="0.35">
@@ -27745,7 +27749,7 @@
         <v>"Mode to directly parallel branch, return index or 0 if none."</v>
       </c>
       <c r="I838" s="1" t="s">
-        <v>1438</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="839" spans="1:9" x14ac:dyDescent="0.35">
@@ -27772,7 +27776,7 @@
         <v>"Set as active load the first load at the active branch, return index or 0 if none."</v>
       </c>
       <c r="I839" s="1" t="s">
-        <v>1439</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="840" spans="1:9" x14ac:dyDescent="0.35">
@@ -27799,7 +27803,7 @@
         <v>"Set as active load the next load at the active branch, return index or 0 if none."</v>
       </c>
       <c r="I840" s="1" t="s">
-        <v>1440</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="841" spans="1:9" x14ac:dyDescent="0.35">
@@ -27826,7 +27830,7 @@
         <v>"Get the topological depth of the active branch."</v>
       </c>
       <c r="I841" s="1" t="s">
-        <v>1441</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="842" spans="1:9" x14ac:dyDescent="0.35">
@@ -27853,7 +27857,7 @@
         <v>"Get the name of the active branch."</v>
       </c>
       <c r="I842" s="1" t="s">
-        <v>1442</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="843" spans="1:9" x14ac:dyDescent="0.35">
@@ -27880,7 +27884,7 @@
         <v>"Set the name of the active branch."</v>
       </c>
       <c r="I843" s="1" t="s">
-        <v>1443</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="844" spans="1:9" x14ac:dyDescent="0.35">
@@ -27907,7 +27911,7 @@
         <v>"Get the name of the active Bus."</v>
       </c>
       <c r="I844" s="1" t="s">
-        <v>1444</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="845" spans="1:9" x14ac:dyDescent="0.35">
@@ -27934,7 +27938,7 @@
         <v>"Set the Bus active by name."</v>
       </c>
       <c r="I845" s="1" t="s">
-        <v>1445</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="846" spans="1:9" x14ac:dyDescent="0.35">
@@ -27961,7 +27965,7 @@
         <v>"Get a vector of all looped element names, by pairs."</v>
       </c>
       <c r="I846" s="1" t="s">
-        <v>1446</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="847" spans="1:9" x14ac:dyDescent="0.35">
@@ -27988,7 +27992,7 @@
         <v>"Get a vector of all isolated branch names."</v>
       </c>
       <c r="I847" s="1" t="s">
-        <v>1447</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="848" spans="1:9" x14ac:dyDescent="0.35">
@@ -28015,7 +28019,7 @@
         <v>"Get a vector of all isolated load names."</v>
       </c>
       <c r="I848" s="1" t="s">
-        <v>1448</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="849" spans="1:9" x14ac:dyDescent="0.35">
@@ -28042,7 +28046,7 @@
         <v>"Get the number of windings on this transformer. Allocates memory; set or change this property first."</v>
       </c>
       <c r="I849" s="1" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="850" spans="1:9" x14ac:dyDescent="0.35">
@@ -28069,7 +28073,7 @@
         <v>"Set the number of windings on this transformer. Allocates memory; set or change this property first."</v>
       </c>
       <c r="I850" s="1" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="851" spans="1:9" x14ac:dyDescent="0.35">
@@ -28096,7 +28100,7 @@
         <v>"Get the active winding number from 1..NumWindings. Update this before reading or setting a sequence of winding properties (R, Tap, kV, kVA, etc.)."</v>
       </c>
       <c r="I851" s="1" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="852" spans="1:9" x14ac:dyDescent="0.35">
@@ -28123,7 +28127,7 @@
         <v>"Set the active winding number from 1..NumWindings. Update this before reading or setting a sequence of winding properties (R, Tap, kV, kVA, etc.)."</v>
       </c>
       <c r="I852" s="1" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="853" spans="1:9" x14ac:dyDescent="0.35">
@@ -28150,7 +28154,7 @@
         <v>"Get the active winding number of tap steps between MinTap and MaxTap."</v>
       </c>
       <c r="I853" s="1" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="854" spans="1:9" x14ac:dyDescent="0.35">
@@ -28177,7 +28181,7 @@
         <v>"Set the active winding number of tap steps between MinTap and MaxTap"</v>
       </c>
       <c r="I854" s="1" t="s">
-        <v>1454</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="855" spans="1:9" x14ac:dyDescent="0.35">
@@ -28204,7 +28208,7 @@
         <v>"Get the information about if the active winding is delta (1) or wye (0) connection."</v>
       </c>
       <c r="I855" s="1" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="856" spans="1:9" x14ac:dyDescent="0.35">
@@ -28231,7 +28235,7 @@
         <v>"Set the information about if the active winding is delta (1) or wye (0) connection."</v>
       </c>
       <c r="I856" s="1" t="s">
-        <v>1456</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="857" spans="1:9" x14ac:dyDescent="0.35">
@@ -28258,7 +28262,7 @@
         <v>"Set the first Transformer active. Return 0 if no more."</v>
       </c>
       <c r="I857" s="1" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="858" spans="1:9" x14ac:dyDescent="0.35">
@@ -28285,7 +28289,7 @@
         <v>"Set the next Transformer active. Return 0 if no more."</v>
       </c>
       <c r="I858" s="1" t="s">
-        <v>1458</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="859" spans="1:9" x14ac:dyDescent="0.35">
@@ -28312,7 +28316,7 @@
         <v>"Get the number of transformers within the active circuit."</v>
       </c>
       <c r="I859" s="1" t="s">
-        <v>1459</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="860" spans="1:9" x14ac:dyDescent="0.35">
@@ -28339,7 +28343,7 @@
         <v>"Get the active winding resistance in %."</v>
       </c>
       <c r="I860" s="1" t="s">
-        <v>1460</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="861" spans="1:9" x14ac:dyDescent="0.35">
@@ -28366,7 +28370,7 @@
         <v>"Set the active winding resistance in %."</v>
       </c>
       <c r="I861" s="1" t="s">
-        <v>1461</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="862" spans="1:9" x14ac:dyDescent="0.35">
@@ -28393,7 +28397,7 @@
         <v>"Get the active winding tap in per-unit."</v>
       </c>
       <c r="I862" s="1" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="863" spans="1:9" x14ac:dyDescent="0.35">
@@ -28420,7 +28424,7 @@
         <v>"Set the active winding tap in per-unit."</v>
       </c>
       <c r="I863" s="1" t="s">
-        <v>1463</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="864" spans="1:9" x14ac:dyDescent="0.35">
@@ -28447,7 +28451,7 @@
         <v>"Get the active winding minimum tap in per-unit."</v>
       </c>
       <c r="I864" s="1" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="865" spans="1:9" x14ac:dyDescent="0.35">
@@ -28474,7 +28478,7 @@
         <v>"Set the active winding minimum tap in per-unit."</v>
       </c>
       <c r="I865" s="1" t="s">
-        <v>1465</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="866" spans="1:9" x14ac:dyDescent="0.35">
@@ -28501,7 +28505,7 @@
         <v>"Get the active winding maximum tap in per-unit."</v>
       </c>
       <c r="I866" s="1" t="s">
-        <v>1466</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="867" spans="1:9" x14ac:dyDescent="0.35">
@@ -28528,7 +28532,7 @@
         <v>"Set the active winding maximum tap in per-unit."</v>
       </c>
       <c r="I867" s="1" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="868" spans="1:9" x14ac:dyDescent="0.35">
@@ -28555,7 +28559,7 @@
         <v>"Get the active winding kV rating. Phase-phase for 2 or 3 phases, actual winding kV 1 phase transformer."</v>
       </c>
       <c r="I868" s="1" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="869" spans="1:9" x14ac:dyDescent="0.35">
@@ -28582,7 +28586,7 @@
         <v>"Set the active winding kV rating. Phase-phase for 2 or 3 phases, actual winding kV 1 phase transformer."</v>
       </c>
       <c r="I869" s="1" t="s">
-        <v>1469</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="870" spans="1:9" x14ac:dyDescent="0.35">
@@ -28609,7 +28613,7 @@
         <v>"Get the active winding kVA rating. On winding 1, this also determines normal and emergency current ratings for all windings."</v>
       </c>
       <c r="I870" s="1" t="s">
-        <v>1470</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="871" spans="1:9" x14ac:dyDescent="0.35">
@@ -28636,7 +28640,7 @@
         <v>"Set the active winding kVA rating. On winding 1, this also determines normal and emergency current ratings for all windings."</v>
       </c>
       <c r="I871" s="1" t="s">
-        <v>1471</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="872" spans="1:9" x14ac:dyDescent="0.35">
@@ -28663,7 +28667,7 @@
         <v>"Get the active winding neutral reactance [ohms] for wye connections."</v>
       </c>
       <c r="I872" s="1" t="s">
-        <v>1472</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="873" spans="1:9" x14ac:dyDescent="0.35">
@@ -28690,7 +28694,7 @@
         <v>"Set the active winding neutral reactance [ohms] for wye connections."</v>
       </c>
       <c r="I873" s="1" t="s">
-        <v>1473</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="874" spans="1:9" x14ac:dyDescent="0.35">
@@ -28717,7 +28721,7 @@
         <v>"Get the active winding neutral resistance [ohms] for wye connections. Set less than zero ungrounded wye."</v>
       </c>
       <c r="I874" s="1" t="s">
-        <v>1474</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="875" spans="1:9" x14ac:dyDescent="0.35">
@@ -28744,7 +28748,7 @@
         <v>"Set the active winding neutral resistance [ohms] for wye connections. Set less than zero ungrounded wye."</v>
       </c>
       <c r="I875" s="1" t="s">
-        <v>1475</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="876" spans="1:9" x14ac:dyDescent="0.35">
@@ -28771,7 +28775,7 @@
         <v>"Get the percent reactance between windings 1 and 2, on winding 1 kVA base. Use for 2 winding or 3 winding transformers."</v>
       </c>
       <c r="I876" s="1" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="877" spans="1:9" x14ac:dyDescent="0.35">
@@ -28798,7 +28802,7 @@
         <v>"Set the percent reactance between windings 1 and 2, on winding 1 kVA base. Use for 2 winding or 3 winding transformers."</v>
       </c>
       <c r="I877" s="1" t="s">
-        <v>1477</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="878" spans="1:9" x14ac:dyDescent="0.35">
@@ -28825,7 +28829,7 @@
         <v>"Get the percent reactance between windings 1 and 3, on winding 1 kVA base. Use for 3 winding transformers only."</v>
       </c>
       <c r="I878" s="1" t="s">
-        <v>1478</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="879" spans="1:9" x14ac:dyDescent="0.35">
@@ -28852,7 +28856,7 @@
         <v>"Set the percent reactance between windings 1 and 3, on winding 1 kVA base. Use for 3 winding transformers only."</v>
       </c>
       <c r="I879" s="1" t="s">
-        <v>1479</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="880" spans="1:9" x14ac:dyDescent="0.35">
@@ -28879,7 +28883,7 @@
         <v>"Get the percent reactance between windings 2 and 3, on winding 1 kVA base. Use for 3 winding transformers only."</v>
       </c>
       <c r="I880" s="1" t="s">
-        <v>1480</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="881" spans="1:9" x14ac:dyDescent="0.35">
@@ -28906,7 +28910,7 @@
         <v>"Set the percent reactance between windings 2 and 3, on winding 1 kVA base. Use for 3 winding transformers only."</v>
       </c>
       <c r="I881" s="1" t="s">
-        <v>1481</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="882" spans="1:9" x14ac:dyDescent="0.35">
@@ -28933,7 +28937,7 @@
         <v>"Get the name of an XfrmCode that supplies electrical parameters for this transformer."</v>
       </c>
       <c r="I882" s="1" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="883" spans="1:9" x14ac:dyDescent="0.35">
@@ -28960,7 +28964,7 @@
         <v>"Set the name of an XfrmCode that supplies electrical parameters for this transformer."</v>
       </c>
       <c r="I883" s="1" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="884" spans="1:9" x14ac:dyDescent="0.35">
@@ -28987,7 +28991,7 @@
         <v>"Get the active transformer name and 3, on winding_1_kVA base. Use for 3 winding transformer only."</v>
       </c>
       <c r="I884" s="1" t="s">
-        <v>1484</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="885" spans="1:9" x14ac:dyDescent="0.35">
@@ -29014,7 +29018,7 @@
         <v>"Set the active transformer name and 3, on winding_1_kVA base. Use for 3 winding transformer only."</v>
       </c>
       <c r="I885" s="1" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="886" spans="1:9" x14ac:dyDescent="0.35">
@@ -29041,7 +29045,7 @@
         <v>"Get a vector of strings with all Transformer names in the active circuit."</v>
       </c>
       <c r="I886" s="1" t="s">
-        <v>1486</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="887" spans="1:9" x14ac:dyDescent="0.35">
@@ -29068,7 +29072,7 @@
         <v>"The number of VSource objects currently defined in the active circuit."</v>
       </c>
       <c r="I887" s="1" t="s">
-        <v>1487</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="888" spans="1:9" x14ac:dyDescent="0.35">
@@ -29095,7 +29099,7 @@
         <v>"Set the first VSource to be active; returns 0 if none."</v>
       </c>
       <c r="I888" s="1" t="s">
-        <v>1488</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="889" spans="1:9" x14ac:dyDescent="0.35">
@@ -29122,7 +29126,7 @@
         <v>"Set the next VSource to be active; returns 0 if none."</v>
       </c>
       <c r="I889" s="1" t="s">
-        <v>1489</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="890" spans="1:9" x14ac:dyDescent="0.35">
@@ -29149,7 +29153,7 @@
         <v>"Get the number of phases of the active VSource."</v>
       </c>
       <c r="I890" s="1" t="s">
-        <v>1490</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="891" spans="1:9" x14ac:dyDescent="0.35">
@@ -29176,7 +29180,7 @@
         <v>"Set the number of phases of the active VSource."</v>
       </c>
       <c r="I891" s="1" t="s">
-        <v>1491</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="892" spans="1:9" x14ac:dyDescent="0.35">
@@ -29203,7 +29207,7 @@
         <v>"Get the source voltage in kV."</v>
       </c>
       <c r="I892" s="1" t="s">
-        <v>1492</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="893" spans="1:9" x14ac:dyDescent="0.35">
@@ -29230,7 +29234,7 @@
         <v>"Set the source voltage in kV."</v>
       </c>
       <c r="I893" s="1" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="894" spans="1:9" x14ac:dyDescent="0.35">
@@ -29257,7 +29261,7 @@
         <v>"Get the source voltage in pu."</v>
       </c>
       <c r="I894" s="1" t="s">
-        <v>1494</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="895" spans="1:9" x14ac:dyDescent="0.35">
@@ -29284,7 +29288,7 @@
         <v>"Set the source voltage in pu."</v>
       </c>
       <c r="I895" s="1" t="s">
-        <v>1495</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="896" spans="1:9" x14ac:dyDescent="0.35">
@@ -29311,7 +29315,7 @@
         <v>"Get the source phase angle of first phase in degrees."</v>
       </c>
       <c r="I896" s="1" t="s">
-        <v>1496</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="897" spans="1:9" x14ac:dyDescent="0.35">
@@ -29338,7 +29342,7 @@
         <v>"Set the source phase angle of first phase in degrees."</v>
       </c>
       <c r="I897" s="1" t="s">
-        <v>1497</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="898" spans="1:9" x14ac:dyDescent="0.35">
@@ -29361,11 +29365,11 @@
         <v>463</v>
       </c>
       <c r="G898" s="1" t="str">
-        <f t="shared" ref="G898:G925" si="14">""""&amp;TRIM(I898)&amp;""""</f>
+        <f t="shared" si="13"/>
         <v>"Get the source frequency in Hz."</v>
       </c>
       <c r="I898" s="1" t="s">
-        <v>1498</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="899" spans="1:9" x14ac:dyDescent="0.35">
@@ -29388,11 +29392,11 @@
         <v>463</v>
       </c>
       <c r="G899" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="G899:G925" si="14">""""&amp;TRIM(I899)&amp;""""</f>
         <v>"Set the source frequency in Hz."</v>
       </c>
       <c r="I899" s="1" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="900" spans="1:9" x14ac:dyDescent="0.35">
@@ -29419,7 +29423,7 @@
         <v>"Get the name of the active VSource."</v>
       </c>
       <c r="I900" s="1" t="s">
-        <v>1500</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="901" spans="1:9" x14ac:dyDescent="0.35">
@@ -29446,7 +29450,7 @@
         <v>"Set the name of the active VSource."</v>
       </c>
       <c r="I901" s="1" t="s">
-        <v>1501</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="902" spans="1:9" x14ac:dyDescent="0.35">
@@ -29473,7 +29477,7 @@
         <v>"Get the names of all Vsources"</v>
       </c>
       <c r="I902" s="1" t="s">
-        <v>1502</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="903" spans="1:9" x14ac:dyDescent="0.35">
@@ -29500,7 +29504,7 @@
         <v>"Get number of XYCurves in active circuit."</v>
       </c>
       <c r="I903" s="1" t="s">
-        <v>1503</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="904" spans="1:9" x14ac:dyDescent="0.35">
@@ -29527,7 +29531,7 @@
         <v>"Set first XYCurves object active; returns 0 if none."</v>
       </c>
       <c r="I904" s="1" t="s">
-        <v>1504</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="905" spans="1:9" x14ac:dyDescent="0.35">
@@ -29554,7 +29558,7 @@
         <v>"Set next XYCurves object active; returns 0 if none."</v>
       </c>
       <c r="I905" s="1" t="s">
-        <v>1505</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="906" spans="1:9" x14ac:dyDescent="0.35">
@@ -29581,7 +29585,7 @@
         <v>"Get the number of points in X-Y curve."</v>
       </c>
       <c r="I906" s="1" t="s">
-        <v>1506</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="907" spans="1:9" x14ac:dyDescent="0.35">
@@ -29608,7 +29612,7 @@
         <v>"Set the number of points in X-Y curve."</v>
       </c>
       <c r="I907" s="1" t="s">
-        <v>1507</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="908" spans="1:9" x14ac:dyDescent="0.35">
@@ -29635,7 +29639,7 @@
         <v>"Get the interpolated value after setting Y."</v>
       </c>
       <c r="I908" s="1" t="s">
-        <v>1508</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="909" spans="1:9" x14ac:dyDescent="0.35">
@@ -29662,7 +29666,7 @@
         <v>"Set the X value."</v>
       </c>
       <c r="I909" s="1" t="s">
-        <v>1509</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="910" spans="1:9" x14ac:dyDescent="0.35">
@@ -29689,7 +29693,7 @@
         <v>"Get the interpolated value after setting X."</v>
       </c>
       <c r="I910" s="1" t="s">
-        <v>1510</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="911" spans="1:9" x14ac:dyDescent="0.35">
@@ -29716,7 +29720,7 @@
         <v>"Set the Y value."</v>
       </c>
       <c r="I911" s="1" t="s">
-        <v>1511</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="912" spans="1:9" x14ac:dyDescent="0.35">
@@ -29743,7 +29747,7 @@
         <v>"Get the amount to shift X value from original curve."</v>
       </c>
       <c r="I912" s="1" t="s">
-        <v>1512</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="913" spans="1:9" x14ac:dyDescent="0.35">
@@ -29770,7 +29774,7 @@
         <v>"Set the amount to shift X value from original curve."</v>
       </c>
       <c r="I913" s="1" t="s">
-        <v>1513</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="914" spans="1:9" x14ac:dyDescent="0.35">
@@ -29797,7 +29801,7 @@
         <v>"Get the amount to shift Y value from original curve."</v>
       </c>
       <c r="I914" s="1" t="s">
-        <v>1514</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="915" spans="1:9" x14ac:dyDescent="0.35">
@@ -29824,7 +29828,7 @@
         <v>"Set the amount to shift Y value from original curve."</v>
       </c>
       <c r="I915" s="1" t="s">
-        <v>1515</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="916" spans="1:9" x14ac:dyDescent="0.35">
@@ -29851,7 +29855,7 @@
         <v>"Get the factor to scale X values from original curve."</v>
       </c>
       <c r="I916" s="1" t="s">
-        <v>1516</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="917" spans="1:9" x14ac:dyDescent="0.35">
@@ -29878,7 +29882,7 @@
         <v>"Set the factor to scale X values from original curve."</v>
       </c>
       <c r="I917" s="1" t="s">
-        <v>1517</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="918" spans="1:9" x14ac:dyDescent="0.35">
@@ -29905,7 +29909,7 @@
         <v>"Get the factor to scale Y values from original curve."</v>
       </c>
       <c r="I918" s="1" t="s">
-        <v>1518</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="919" spans="1:9" x14ac:dyDescent="0.35">
@@ -29932,7 +29936,7 @@
         <v>"Set the factor to scale Y values from original curve."</v>
       </c>
       <c r="I919" s="1" t="s">
-        <v>1519</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="920" spans="1:9" x14ac:dyDescent="0.35">
@@ -29959,7 +29963,7 @@
         <v>"Get the name of the active XYCurve Object."</v>
       </c>
       <c r="I920" s="1" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="921" spans="1:9" x14ac:dyDescent="0.35">
@@ -29986,7 +29990,7 @@
         <v>"Set the name of the active XYCurve Object."</v>
       </c>
       <c r="I921" s="1" t="s">
-        <v>1521</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="922" spans="1:9" x14ac:dyDescent="0.35">
@@ -30013,7 +30017,7 @@
         <v>"Get the X values as a vector of doubles. Set Npts to max number expected if setting."</v>
       </c>
       <c r="I922" s="1" t="s">
-        <v>1522</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="923" spans="1:9" x14ac:dyDescent="0.35">
@@ -30040,7 +30044,7 @@
         <v>"Set the X values as a vector of doubles. Set Npts to max number expected if setting"</v>
       </c>
       <c r="I923" s="1" t="s">
-        <v>1523</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="924" spans="1:9" x14ac:dyDescent="0.35">
@@ -30067,7 +30071,7 @@
         <v>"Get the Y values as a vector of doubles. Set Npts to max number expected if setting."</v>
       </c>
       <c r="I924" s="1" t="s">
-        <v>1524</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="925" spans="1:9" x14ac:dyDescent="0.35">
@@ -30094,7 +30098,7 @@
         <v>"Set the Y values as a vector of doubles. Set Npts to max number expected if setting"</v>
       </c>
       <c r="I925" s="1" t="s">
-        <v>1525</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="926" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Change DSS API to use functions in modules
</commit_message>
<xml_diff>
--- a/src/api.xlsx
+++ b/src/api.xlsx
@@ -4996,13 +4996,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I959"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A545" workbookViewId="0">
-      <selection activeCell="A582" sqref="A582:H583"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.7109375" style="1"/>
+    <col min="1" max="2" width="8.7109375" style="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" style="1"/>
     <col min="6" max="6" width="17.42578125" style="1" customWidth="1"/>

</xml_diff>